<commit_message>
Added NLCD>MapShed table to bottom of TechDocs
Partially resolves #9, Add "NLCD to MapShed land class" lookup table.
Added table is not used as a lookup.
Also, uses MMW v1.23 mapping of "NLCD 21 Developed, Open Space", described in https://github.com/WikiWatershed/model-my-watershed/issues/2937.
Need to upgrade with MMW release 1.24
</commit_message>
<xml_diff>
--- a/MMW_BMP_Spreadsheet_Tool.xlsx
+++ b/MMW_BMP_Spreadsheet_Tool.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaufdenkampe/Google Drive/WikiWatershed/ModelMyWatershed2-WPF-Project/MMW-BMPs/Barry/MMW-BMP-Tool_update_2018-10-03/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaufdenkampe/Documents/GitHub/MMW-BMP-spreadsheet-tool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D24EB65-D48F-E449-B6CA-FA2C8BDD677F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC7B525-CAB3-554D-996B-F92840703093}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2780" yWindow="-21140" windowWidth="32720" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2640" yWindow="-21140" windowWidth="22540" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="14" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="551">
   <si>
     <t>Load Reductions from BMP Implementation in Urban and Rural Areas</t>
   </si>
@@ -1843,7 +1843,79 @@
     <t>Section 2: Landcover Loading Rates Look-Up Table</t>
   </si>
   <si>
-    <t>2018-10-03 at 9:00am ET</t>
+    <t>Land Cover: NLCD2011 --&gt; MapShed</t>
+  </si>
+  <si>
+    <t>NLCD Code</t>
+  </si>
+  <si>
+    <t>NLCD name</t>
+  </si>
+  <si>
+    <t>MapShed Code</t>
+  </si>
+  <si>
+    <t>Land Use term in GMS file</t>
+  </si>
+  <si>
+    <t>Mapshed Source List Order</t>
+  </si>
+  <si>
+    <t>Mapshed Source Terms</t>
+  </si>
+  <si>
+    <t>MMW Source List Order</t>
+  </si>
+  <si>
+    <t>MMW Source Terms (v1.23.0)</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Ld_Open_Space (formerly Ld_Residential)</t>
+  </si>
+  <si>
+    <t>Low-Density Open Space</t>
+  </si>
+  <si>
+    <t>Dwarf Scrub</t>
+  </si>
+  <si>
+    <t>NA – Alaska only</t>
+  </si>
+  <si>
+    <t>Sedge/Herbaceous</t>
+  </si>
+  <si>
+    <t>Lichens</t>
+  </si>
+  <si>
+    <t>Moss</t>
+  </si>
+  <si>
+    <t>https://www.mrlc.gov/nlcd11_leg.php</t>
+  </si>
+  <si>
+    <t>NLCD Legend:</t>
+  </si>
+  <si>
+    <t>The National Land Cover Database 2011 (NLCD2011) categories are mapped to MapShed/GWLF-E Land Use categories according to the following table.</t>
+  </si>
+  <si>
+    <t>NOTE 1: Some NLCD categories are combined into a single MapShed category, whereas some MapShed categories are left unused.</t>
+  </si>
+  <si>
+    <t>NOTE 2: Curve numbers for MMW are generated from the Impervious Surface percentages estimated from NLCD, and given above.</t>
+  </si>
+  <si>
+    <t>2018-10-03 at 3:19 pm CT</t>
+  </si>
+  <si>
+    <t>NOTE: For MMW versions &gt;-=v1.24</t>
+  </si>
+  <si>
+    <t>NOTE: For MMW versions &lt;=v1.23</t>
   </si>
 </sst>
 </file>
@@ -1860,7 +1932,7 @@
     <numFmt numFmtId="169" formatCode="0.000"/>
     <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="91">
+  <fonts count="93">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2500,6 +2572,20 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="48">
@@ -3926,7 +4012,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="566">
+  <cellXfs count="576">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -5067,6 +5153,26 @@
     <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="53" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5157,6 +5263,36 @@
     <xf numFmtId="0" fontId="90" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="92" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="93" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="4" fontId="26" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="26" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="26" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5191,36 +5327,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="4" fontId="26" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="26" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="26" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="90" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="92" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="93" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="4" fontId="52" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8082,7 +8188,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
@@ -8123,7 +8231,7 @@
         <v>469</v>
       </c>
       <c r="C4" s="442" t="s">
-        <v>526</v>
+        <v>548</v>
       </c>
       <c r="E4" s="443"/>
       <c r="F4" s="438"/>
@@ -8217,36 +8325,36 @@
       <c r="I14" s="438"/>
     </row>
     <row r="15" spans="1:12" s="449" customFormat="1" ht="45" customHeight="1">
-      <c r="A15" s="508" t="s">
+      <c r="A15" s="518" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="508"/>
-      <c r="C15" s="508"/>
-      <c r="D15" s="508"/>
-      <c r="E15" s="508"/>
-      <c r="F15" s="508"/>
-      <c r="G15" s="508"/>
-      <c r="H15" s="508"/>
-      <c r="I15" s="508"/>
-      <c r="J15" s="508"/>
-      <c r="K15" s="508"/>
-      <c r="L15" s="508"/>
+      <c r="B15" s="518"/>
+      <c r="C15" s="518"/>
+      <c r="D15" s="518"/>
+      <c r="E15" s="518"/>
+      <c r="F15" s="518"/>
+      <c r="G15" s="518"/>
+      <c r="H15" s="518"/>
+      <c r="I15" s="518"/>
+      <c r="J15" s="518"/>
+      <c r="K15" s="518"/>
+      <c r="L15" s="518"/>
     </row>
     <row r="16" spans="1:12" s="449" customFormat="1" ht="51.75" customHeight="1">
-      <c r="A16" s="508" t="s">
+      <c r="A16" s="518" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="508"/>
-      <c r="C16" s="508"/>
-      <c r="D16" s="508"/>
-      <c r="E16" s="508"/>
-      <c r="F16" s="508"/>
-      <c r="G16" s="508"/>
-      <c r="H16" s="508"/>
-      <c r="I16" s="508"/>
-      <c r="J16" s="508"/>
-      <c r="K16" s="508"/>
-      <c r="L16" s="508"/>
+      <c r="B16" s="518"/>
+      <c r="C16" s="518"/>
+      <c r="D16" s="518"/>
+      <c r="E16" s="518"/>
+      <c r="F16" s="518"/>
+      <c r="G16" s="518"/>
+      <c r="H16" s="518"/>
+      <c r="I16" s="518"/>
+      <c r="J16" s="518"/>
+      <c r="K16" s="518"/>
+      <c r="L16" s="518"/>
     </row>
     <row r="17" spans="1:12" ht="16">
       <c r="B17" s="448"/>
@@ -8268,52 +8376,52 @@
       <c r="I18" s="438"/>
     </row>
     <row r="19" spans="1:12" s="450" customFormat="1" ht="70.5" customHeight="1">
-      <c r="A19" s="506" t="s">
+      <c r="A19" s="516" t="s">
         <v>474</v>
       </c>
-      <c r="B19" s="506"/>
-      <c r="C19" s="506"/>
-      <c r="D19" s="506"/>
-      <c r="E19" s="506"/>
-      <c r="F19" s="506"/>
-      <c r="G19" s="506"/>
-      <c r="H19" s="506"/>
-      <c r="I19" s="506"/>
-      <c r="J19" s="506"/>
-      <c r="K19" s="506"/>
-      <c r="L19" s="506"/>
+      <c r="B19" s="516"/>
+      <c r="C19" s="516"/>
+      <c r="D19" s="516"/>
+      <c r="E19" s="516"/>
+      <c r="F19" s="516"/>
+      <c r="G19" s="516"/>
+      <c r="H19" s="516"/>
+      <c r="I19" s="516"/>
+      <c r="J19" s="516"/>
+      <c r="K19" s="516"/>
+      <c r="L19" s="516"/>
     </row>
     <row r="20" spans="1:12" s="450" customFormat="1" ht="63.75" customHeight="1">
-      <c r="A20" s="509" t="s">
+      <c r="A20" s="519" t="s">
         <v>471</v>
       </c>
-      <c r="B20" s="509"/>
-      <c r="C20" s="509"/>
-      <c r="D20" s="509"/>
-      <c r="E20" s="509"/>
-      <c r="F20" s="509"/>
-      <c r="G20" s="509"/>
-      <c r="H20" s="509"/>
-      <c r="I20" s="509"/>
-      <c r="J20" s="509"/>
-      <c r="K20" s="509"/>
-      <c r="L20" s="509"/>
+      <c r="B20" s="519"/>
+      <c r="C20" s="519"/>
+      <c r="D20" s="519"/>
+      <c r="E20" s="519"/>
+      <c r="F20" s="519"/>
+      <c r="G20" s="519"/>
+      <c r="H20" s="519"/>
+      <c r="I20" s="519"/>
+      <c r="J20" s="519"/>
+      <c r="K20" s="519"/>
+      <c r="L20" s="519"/>
     </row>
     <row r="21" spans="1:12" s="450" customFormat="1" ht="94.5" customHeight="1">
-      <c r="A21" s="509" t="s">
+      <c r="A21" s="519" t="s">
         <v>472</v>
       </c>
-      <c r="B21" s="509"/>
-      <c r="C21" s="509"/>
-      <c r="D21" s="509"/>
-      <c r="E21" s="509"/>
-      <c r="F21" s="509"/>
-      <c r="G21" s="509"/>
-      <c r="H21" s="509"/>
-      <c r="I21" s="509"/>
-      <c r="J21" s="509"/>
-      <c r="K21" s="509"/>
-      <c r="L21" s="509"/>
+      <c r="B21" s="519"/>
+      <c r="C21" s="519"/>
+      <c r="D21" s="519"/>
+      <c r="E21" s="519"/>
+      <c r="F21" s="519"/>
+      <c r="G21" s="519"/>
+      <c r="H21" s="519"/>
+      <c r="I21" s="519"/>
+      <c r="J21" s="519"/>
+      <c r="K21" s="519"/>
+      <c r="L21" s="519"/>
     </row>
     <row r="22" spans="1:12" s="450" customFormat="1" ht="16">
       <c r="A22" s="451" t="s">
@@ -8413,20 +8521,20 @@
       <c r="E31" s="444"/>
     </row>
     <row r="32" spans="1:12" ht="101.25" customHeight="1">
-      <c r="A32" s="506" t="s">
+      <c r="A32" s="516" t="s">
         <v>500</v>
       </c>
-      <c r="B32" s="507"/>
-      <c r="C32" s="507"/>
-      <c r="D32" s="507"/>
-      <c r="E32" s="507"/>
-      <c r="F32" s="507"/>
-      <c r="G32" s="507"/>
-      <c r="H32" s="507"/>
-      <c r="I32" s="507"/>
-      <c r="J32" s="507"/>
-      <c r="K32" s="507"/>
-      <c r="L32" s="507"/>
+      <c r="B32" s="517"/>
+      <c r="C32" s="517"/>
+      <c r="D32" s="517"/>
+      <c r="E32" s="517"/>
+      <c r="F32" s="517"/>
+      <c r="G32" s="517"/>
+      <c r="H32" s="517"/>
+      <c r="I32" s="517"/>
+      <c r="J32" s="517"/>
+      <c r="K32" s="517"/>
+      <c r="L32" s="517"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -8456,10 +8564,10 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
-  <dimension ref="A1:T157"/>
+  <dimension ref="A1:T197"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="M181" sqref="M181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -11277,38 +11385,797 @@
       <c r="S156" s="246"/>
       <c r="T156" s="246"/>
     </row>
-    <row r="157" spans="1:20">
-      <c r="A157" s="246"/>
-      <c r="B157" s="246"/>
-      <c r="C157" s="246"/>
-      <c r="D157" s="246"/>
-      <c r="E157" s="246"/>
-      <c r="F157" s="246"/>
-      <c r="G157" s="246"/>
-      <c r="H157" s="246"/>
-      <c r="I157" s="246"/>
-      <c r="J157" s="246"/>
-      <c r="R157" s="246"/>
-      <c r="S157" s="246"/>
-      <c r="T157" s="246"/>
+    <row r="157" spans="1:20" ht="31">
+      <c r="A157" s="485" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="158" spans="1:20">
+      <c r="A158" s="509" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="159" spans="1:20">
+      <c r="A159" s="509" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="160" spans="1:20">
+      <c r="A160" s="509" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" ht="16">
+      <c r="A161" s="509" t="s">
+        <v>544</v>
+      </c>
+      <c r="B161" s="338" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" s="3" customFormat="1" ht="57">
+      <c r="A162" s="510" t="s">
+        <v>527</v>
+      </c>
+      <c r="B162" s="511" t="s">
+        <v>528</v>
+      </c>
+      <c r="C162" s="510" t="s">
+        <v>529</v>
+      </c>
+      <c r="D162" s="510" t="s">
+        <v>530</v>
+      </c>
+      <c r="E162" s="510" t="s">
+        <v>531</v>
+      </c>
+      <c r="F162" s="510" t="s">
+        <v>532</v>
+      </c>
+      <c r="G162" s="510" t="s">
+        <v>533</v>
+      </c>
+      <c r="H162" s="515" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
+      <c r="A163" s="506">
+        <v>11</v>
+      </c>
+      <c r="B163" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C163" s="506">
+        <v>1</v>
+      </c>
+      <c r="D163" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E163" s="7"/>
+      <c r="F163" s="7"/>
+      <c r="G163" s="7"/>
+      <c r="H163" s="7"/>
+    </row>
+    <row r="164" spans="1:11">
+      <c r="A164" s="506">
+        <v>12</v>
+      </c>
+      <c r="B164" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C164" s="506">
+        <v>22</v>
+      </c>
+      <c r="D164" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E164" s="7">
+        <v>8</v>
+      </c>
+      <c r="F164" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G164" s="7">
+        <v>6</v>
+      </c>
+      <c r="H164" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11">
+      <c r="A165" s="506">
+        <v>21</v>
+      </c>
+      <c r="B165" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C165" s="508" t="s">
+        <v>535</v>
+      </c>
+      <c r="D165" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="E165" s="507">
+        <v>11</v>
+      </c>
+      <c r="F165" s="507" t="s">
+        <v>46</v>
+      </c>
+      <c r="G165" s="507">
+        <v>7</v>
+      </c>
+      <c r="H165" s="507" t="s">
+        <v>110</v>
+      </c>
+      <c r="K165" s="334" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11">
+      <c r="A166" s="506">
+        <v>22</v>
+      </c>
+      <c r="B166" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C166" s="506">
+        <v>2</v>
+      </c>
+      <c r="D166" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E166" s="7">
+        <v>11</v>
+      </c>
+      <c r="F166" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G166" s="7">
+        <v>7</v>
+      </c>
+      <c r="H166" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11">
+      <c r="A167" s="506">
+        <v>23</v>
+      </c>
+      <c r="B167" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C167" s="506">
+        <v>20</v>
+      </c>
+      <c r="D167" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E167" s="7">
+        <v>12</v>
+      </c>
+      <c r="F167" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G167" s="7">
+        <v>8</v>
+      </c>
+      <c r="H167" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11">
+      <c r="A168" s="506">
+        <v>24</v>
+      </c>
+      <c r="B168" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C168" s="506">
+        <v>3</v>
+      </c>
+      <c r="D168" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E168" s="7">
+        <v>13</v>
+      </c>
+      <c r="F168" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G168" s="7">
+        <v>9</v>
+      </c>
+      <c r="H168" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11">
+      <c r="A169" s="506">
+        <v>31</v>
+      </c>
+      <c r="B169" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C169" s="506">
+        <v>22</v>
+      </c>
+      <c r="D169" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E169" s="7">
+        <v>8</v>
+      </c>
+      <c r="F169" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G169" s="7">
+        <v>6</v>
+      </c>
+      <c r="H169" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11">
+      <c r="A170" s="506">
+        <v>41</v>
+      </c>
+      <c r="B170" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C170" s="506">
+        <v>7</v>
+      </c>
+      <c r="D170" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E170" s="7">
+        <v>3</v>
+      </c>
+      <c r="F170" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G170" s="7">
+        <v>3</v>
+      </c>
+      <c r="H170" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11">
+      <c r="A171" s="506">
+        <v>42</v>
+      </c>
+      <c r="B171" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C171" s="506">
+        <v>8</v>
+      </c>
+      <c r="D171" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E171" s="7">
+        <v>3</v>
+      </c>
+      <c r="F171" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G171" s="7">
+        <v>3</v>
+      </c>
+      <c r="H171" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11">
+      <c r="A172" s="506">
+        <v>43</v>
+      </c>
+      <c r="B172" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C172" s="506">
+        <v>9</v>
+      </c>
+      <c r="D172" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E172" s="7">
+        <v>3</v>
+      </c>
+      <c r="F172" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G172" s="7">
+        <v>3</v>
+      </c>
+      <c r="H172" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11">
+      <c r="A173" s="506">
+        <v>51</v>
+      </c>
+      <c r="B173" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="C173" s="506" t="s">
+        <v>539</v>
+      </c>
+      <c r="D173" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E173" s="7"/>
+      <c r="F173" s="7"/>
+      <c r="G173" s="7"/>
+      <c r="H173" s="7"/>
+    </row>
+    <row r="174" spans="1:11">
+      <c r="A174" s="506">
+        <v>52</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C174" s="506">
+        <v>9</v>
+      </c>
+      <c r="D174" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E174" s="7">
+        <v>3</v>
+      </c>
+      <c r="F174" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G174" s="7">
+        <v>3</v>
+      </c>
+      <c r="H174" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11">
+      <c r="A175" s="506">
+        <v>71</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C175" s="506">
+        <v>21</v>
+      </c>
+      <c r="D175" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E175" s="7">
+        <v>7</v>
+      </c>
+      <c r="F175" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G175" s="7">
+        <v>5</v>
+      </c>
+      <c r="H175" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11">
+      <c r="A176" s="506">
+        <v>72</v>
+      </c>
+      <c r="B176" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="C176" s="506" t="s">
+        <v>539</v>
+      </c>
+      <c r="D176" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E176" s="7"/>
+      <c r="F176" s="7"/>
+      <c r="G176" s="7"/>
+      <c r="H176" s="7"/>
+    </row>
+    <row r="177" spans="1:11">
+      <c r="A177" s="506">
+        <v>73</v>
+      </c>
+      <c r="B177" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="C177" s="506" t="s">
+        <v>539</v>
+      </c>
+      <c r="D177" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E177" s="7"/>
+      <c r="F177" s="7"/>
+      <c r="G177" s="7"/>
+      <c r="H177" s="7"/>
+    </row>
+    <row r="178" spans="1:11">
+      <c r="A178" s="506">
+        <v>74</v>
+      </c>
+      <c r="B178" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="C178" s="506" t="s">
+        <v>539</v>
+      </c>
+      <c r="D178" s="7" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="E178" s="7"/>
+      <c r="F178" s="7"/>
+      <c r="G178" s="7"/>
+      <c r="H178" s="7"/>
+    </row>
+    <row r="179" spans="1:11">
+      <c r="A179" s="506">
+        <v>81</v>
+      </c>
+      <c r="B179" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C179" s="506">
+        <v>4</v>
+      </c>
+      <c r="D179" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E179" s="7">
+        <v>1</v>
+      </c>
+      <c r="F179" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G179" s="7">
+        <v>1</v>
+      </c>
+      <c r="H179" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11">
+      <c r="A180" s="506">
+        <v>82</v>
+      </c>
+      <c r="B180" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C180" s="506">
+        <v>5</v>
+      </c>
+      <c r="D180" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E180" s="7">
+        <v>2</v>
+      </c>
+      <c r="F180" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G180" s="7">
+        <v>2</v>
+      </c>
+      <c r="H180" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11">
+      <c r="A181" s="506">
+        <v>90</v>
+      </c>
+      <c r="B181" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C181" s="506">
+        <v>10</v>
+      </c>
+      <c r="D181" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E181" s="7">
+        <v>4</v>
+      </c>
+      <c r="F181" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G181" s="7">
+        <v>4</v>
+      </c>
+      <c r="H181" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11">
+      <c r="A182" s="506">
+        <v>95</v>
+      </c>
+      <c r="B182" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C182" s="506">
+        <v>11</v>
+      </c>
+      <c r="D182" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E182" s="7">
+        <v>4</v>
+      </c>
+      <c r="F182" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G182" s="7">
+        <v>4</v>
+      </c>
+      <c r="H182" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11">
+      <c r="A183" s="7"/>
+      <c r="B183" s="7"/>
+      <c r="C183" s="7"/>
+      <c r="D183" s="7"/>
+      <c r="E183" s="7"/>
+      <c r="F183" s="7"/>
+      <c r="G183" s="7"/>
+      <c r="H183" s="7"/>
+    </row>
+    <row r="184" spans="1:11">
+      <c r="A184" s="7"/>
+      <c r="B184" s="7"/>
+      <c r="C184" s="7"/>
+      <c r="D184" s="7"/>
+      <c r="E184" s="7">
+        <v>9</v>
+      </c>
+      <c r="F184" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G184" s="7">
+        <v>6</v>
+      </c>
+      <c r="H184" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11">
+      <c r="A185" s="7"/>
+      <c r="B185" s="7"/>
+      <c r="C185" s="7"/>
+      <c r="D185" s="7"/>
+      <c r="E185" s="507">
+        <v>5</v>
+      </c>
+      <c r="F185" s="507" t="s">
+        <v>40</v>
+      </c>
+      <c r="G185" s="507"/>
+      <c r="H185" s="507" t="s">
+        <v>116</v>
+      </c>
+      <c r="K185" s="334" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11">
+      <c r="A186" s="7"/>
+      <c r="B186" s="7"/>
+      <c r="C186" s="7"/>
+      <c r="D186" s="7"/>
+      <c r="E186" s="507">
+        <v>6</v>
+      </c>
+      <c r="F186" s="507" t="s">
+        <v>41</v>
+      </c>
+      <c r="G186" s="507"/>
+      <c r="H186" s="507" t="s">
+        <v>116</v>
+      </c>
+      <c r="K186" s="334" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11">
+      <c r="A187" s="7"/>
+      <c r="B187" s="7"/>
+      <c r="C187" s="7"/>
+      <c r="D187" s="7"/>
+      <c r="E187" s="507">
+        <v>10</v>
+      </c>
+      <c r="F187" s="507" t="s">
+        <v>45</v>
+      </c>
+      <c r="G187" s="507"/>
+      <c r="H187" s="507" t="s">
+        <v>116</v>
+      </c>
+      <c r="K187" s="334" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11">
+      <c r="A188" s="7"/>
+      <c r="B188" s="7"/>
+      <c r="C188" s="7"/>
+      <c r="D188" s="7"/>
+      <c r="E188" s="7">
+        <v>15</v>
+      </c>
+      <c r="F188" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G188" s="7"/>
+      <c r="H188" s="7"/>
+    </row>
+    <row r="189" spans="1:11">
+      <c r="A189" s="7"/>
+      <c r="B189" s="7"/>
+      <c r="C189" s="7"/>
+      <c r="D189" s="7"/>
+      <c r="E189" s="7">
+        <v>16</v>
+      </c>
+      <c r="F189" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G189" s="7"/>
+      <c r="H189" s="7"/>
+    </row>
+    <row r="190" spans="1:11">
+      <c r="A190" s="7"/>
+      <c r="B190" s="7"/>
+      <c r="C190" s="7"/>
+      <c r="D190" s="7"/>
+      <c r="E190" s="7">
+        <v>17</v>
+      </c>
+      <c r="F190" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G190" s="7">
+        <v>11</v>
+      </c>
+      <c r="H190" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11">
+      <c r="A191" s="7"/>
+      <c r="B191" s="7"/>
+      <c r="C191" s="7"/>
+      <c r="D191" s="7"/>
+      <c r="E191" s="7">
+        <v>18</v>
+      </c>
+      <c r="F191" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G191" s="7"/>
+      <c r="H191" s="7"/>
+    </row>
+    <row r="192" spans="1:11">
+      <c r="A192" s="7"/>
+      <c r="B192" s="7"/>
+      <c r="C192" s="7"/>
+      <c r="D192" s="7"/>
+      <c r="E192" s="7">
+        <v>19</v>
+      </c>
+      <c r="F192" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="G192" s="7">
+        <v>12</v>
+      </c>
+      <c r="H192" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11">
+      <c r="A193" s="7"/>
+      <c r="B193" s="7"/>
+      <c r="C193" s="7"/>
+      <c r="D193" s="7"/>
+      <c r="E193" s="7">
+        <v>20</v>
+      </c>
+      <c r="F193" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G193" s="7">
+        <v>13</v>
+      </c>
+      <c r="H193" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11">
+      <c r="A194" s="7"/>
+      <c r="B194" s="7"/>
+      <c r="C194" s="7"/>
+      <c r="D194" s="7"/>
+      <c r="E194" s="7">
+        <v>21</v>
+      </c>
+      <c r="F194" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G194" s="7">
+        <v>14</v>
+      </c>
+      <c r="H194" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11">
+      <c r="A195" s="7"/>
+      <c r="B195" s="7"/>
+      <c r="C195" s="7"/>
+      <c r="D195" s="7"/>
+      <c r="E195" s="7">
+        <v>22</v>
+      </c>
+      <c r="F195" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G195" s="7">
+        <v>15</v>
+      </c>
+      <c r="H195" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11">
+      <c r="E197" s="513">
+        <v>14</v>
+      </c>
+      <c r="F197" s="513" t="s">
+        <v>49</v>
+      </c>
+      <c r="G197" s="513">
+        <v>10</v>
+      </c>
+      <c r="H197" s="513" t="s">
+        <v>537</v>
+      </c>
+      <c r="I197" s="331"/>
+      <c r="K197" s="514" t="s">
+        <v>549</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K88" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="K87" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
     <hyperlink ref="B80" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B162" r:id="rId4" display="https://www.mrlc.gov/nlcd11_leg.php" xr:uid="{0FAA8ECC-5199-9E4D-8AE4-389AF74FCF76}"/>
+    <hyperlink ref="B161" r:id="rId5" xr:uid="{7F3C85E6-63AD-B140-980F-C108B8B2C347}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;14Look-Up Table: Christina Basin MapShed Land Use Loading Rates</oddHeader>
     <oddFooter>&amp;L&amp;"Arial,Regular"&amp;9Section 1: Instructions and O&amp;Overview&amp;C&amp;"Arial,Regular"&amp;9Page &amp;P of &amp;N&amp;R&amp;"Arial,Regular"&amp;9Christina Basin Loading Rates Tool (May 5, 2017)</oddFooter>
   </headerFooter>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId7"/>
   <tableParts count="3">
-    <tablePart r:id="rId6"/>
-    <tablePart r:id="rId7"/>
     <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
@@ -11322,7 +12189,7 @@
   <dimension ref="A1:P114"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N82" sqref="N82"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -11363,11 +12230,11 @@
       <c r="A3" s="91" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="510">
+      <c r="B3" s="520">
         <f>+C14</f>
         <v>2018</v>
       </c>
-      <c r="C3" s="510"/>
+      <c r="C3" s="520"/>
     </row>
     <row r="5" spans="1:6" s="499" customFormat="1" ht="16">
       <c r="A5" s="498" t="s">
@@ -11378,14 +12245,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="122" customHeight="1">
-      <c r="A7" s="511" t="s">
+      <c r="A7" s="521" t="s">
         <v>524</v>
       </c>
-      <c r="B7" s="511"/>
-      <c r="C7" s="511"/>
-      <c r="D7" s="511"/>
-      <c r="E7" s="511"/>
-      <c r="F7" s="511"/>
+      <c r="B7" s="521"/>
+      <c r="C7" s="521"/>
+      <c r="D7" s="521"/>
+      <c r="E7" s="521"/>
+      <c r="F7" s="521"/>
     </row>
     <row r="8" spans="1:6" ht="14">
       <c r="A8" s="93"/>
@@ -11441,12 +12308,12 @@
       <c r="C15" s="98"/>
     </row>
     <row r="16" spans="1:6" ht="14" thickBot="1">
-      <c r="C16" s="512" t="s">
+      <c r="C16" s="522" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="512"/>
-      <c r="E16" s="512"/>
-      <c r="F16" s="512"/>
+      <c r="D16" s="522"/>
+      <c r="E16" s="522"/>
+      <c r="F16" s="522"/>
     </row>
     <row r="17" spans="1:13" ht="14" thickBot="1"/>
     <row r="18" spans="1:13" ht="14">
@@ -12023,7 +12890,9 @@
       <c r="A47" s="91" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="112"/>
+      <c r="C47" s="112" t="s">
+        <v>527</v>
+      </c>
       <c r="D47" s="91" t="s">
         <v>89</v>
       </c>
@@ -12056,6 +12925,9 @@
       <c r="A48" s="91" t="s">
         <v>98</v>
       </c>
+      <c r="C48" s="512">
+        <v>11</v>
+      </c>
       <c r="D48" s="459">
         <v>0</v>
       </c>
@@ -12092,6 +12964,9 @@
       <c r="A49" s="91" t="s">
         <v>100</v>
       </c>
+      <c r="C49" s="512">
+        <v>12</v>
+      </c>
       <c r="D49" s="459">
         <v>0</v>
       </c>
@@ -12128,6 +13003,9 @@
       <c r="A50" s="91" t="s">
         <v>101</v>
       </c>
+      <c r="C50" s="512">
+        <v>21</v>
+      </c>
       <c r="D50" s="459">
         <v>0</v>
       </c>
@@ -12164,6 +13042,9 @@
       <c r="A51" s="91" t="s">
         <v>103</v>
       </c>
+      <c r="C51" s="512">
+        <v>22</v>
+      </c>
       <c r="D51" s="459">
         <v>0</v>
       </c>
@@ -12200,6 +13081,9 @@
       <c r="A52" s="91" t="s">
         <v>105</v>
       </c>
+      <c r="C52" s="512">
+        <v>23</v>
+      </c>
       <c r="D52" s="459">
         <v>0</v>
       </c>
@@ -12236,6 +13120,9 @@
       <c r="A53" s="91" t="s">
         <v>107</v>
       </c>
+      <c r="C53" s="512">
+        <v>24</v>
+      </c>
       <c r="D53" s="459">
         <v>0</v>
       </c>
@@ -12272,6 +13159,9 @@
       <c r="A54" s="91" t="s">
         <v>109</v>
       </c>
+      <c r="C54" s="512">
+        <v>31</v>
+      </c>
       <c r="D54" s="459">
         <v>0</v>
       </c>
@@ -12308,6 +13198,9 @@
       <c r="A55" s="91" t="s">
         <v>111</v>
       </c>
+      <c r="C55" s="512">
+        <v>41</v>
+      </c>
       <c r="D55" s="459">
         <v>0</v>
       </c>
@@ -12344,6 +13237,9 @@
       <c r="A56" s="91" t="s">
         <v>113</v>
       </c>
+      <c r="C56" s="512">
+        <v>42</v>
+      </c>
       <c r="D56" s="459">
         <v>0</v>
       </c>
@@ -12380,6 +13276,9 @@
       <c r="A57" s="91" t="s">
         <v>115</v>
       </c>
+      <c r="C57" s="512">
+        <v>43</v>
+      </c>
       <c r="D57" s="459">
         <v>0</v>
       </c>
@@ -12416,6 +13315,9 @@
       <c r="A58" s="91" t="s">
         <v>117</v>
       </c>
+      <c r="C58" s="512">
+        <v>52</v>
+      </c>
       <c r="D58" s="459">
         <v>0</v>
       </c>
@@ -12452,6 +13354,9 @@
       <c r="A59" s="91" t="s">
         <v>118</v>
       </c>
+      <c r="C59" s="512">
+        <v>71</v>
+      </c>
       <c r="D59" s="459">
         <v>0</v>
       </c>
@@ -12488,6 +13393,9 @@
       <c r="A60" s="91" t="s">
         <v>120</v>
       </c>
+      <c r="C60" s="512">
+        <v>81</v>
+      </c>
       <c r="D60" s="459">
         <v>0</v>
       </c>
@@ -12524,6 +13432,9 @@
       <c r="A61" s="91" t="s">
         <v>122</v>
       </c>
+      <c r="C61" s="512">
+        <v>82</v>
+      </c>
       <c r="D61" s="459">
         <v>0</v>
       </c>
@@ -12560,6 +13471,9 @@
       <c r="A62" s="91" t="s">
         <v>124</v>
       </c>
+      <c r="C62" s="512">
+        <v>90</v>
+      </c>
       <c r="D62" s="459">
         <v>0</v>
       </c>
@@ -12596,6 +13510,9 @@
       <c r="A63" s="91" t="s">
         <v>125</v>
       </c>
+      <c r="C63" s="512">
+        <v>95</v>
+      </c>
       <c r="D63" s="459">
         <v>0</v>
       </c>
@@ -12658,7 +13575,9 @@
       <c r="A72" s="91" t="s">
         <v>88</v>
       </c>
-      <c r="C72" s="112"/>
+      <c r="C72" s="112" t="s">
+        <v>527</v>
+      </c>
       <c r="D72" s="91" t="s">
         <v>89</v>
       </c>
@@ -12679,6 +13598,9 @@
       <c r="A73" s="91" t="s">
         <v>98</v>
       </c>
+      <c r="C73" s="512">
+        <v>11</v>
+      </c>
       <c r="D73" s="459">
         <v>0</v>
       </c>
@@ -12691,6 +13613,9 @@
       <c r="A74" s="91" t="s">
         <v>100</v>
       </c>
+      <c r="C74" s="512">
+        <v>12</v>
+      </c>
       <c r="D74" s="459">
         <v>0</v>
       </c>
@@ -12703,6 +13628,9 @@
       <c r="A75" s="91" t="s">
         <v>101</v>
       </c>
+      <c r="C75" s="512">
+        <v>21</v>
+      </c>
       <c r="D75" s="459">
         <v>0</v>
       </c>
@@ -12730,6 +13658,9 @@
       <c r="A76" s="91" t="s">
         <v>103</v>
       </c>
+      <c r="C76" s="512">
+        <v>22</v>
+      </c>
       <c r="D76" s="459">
         <v>0</v>
       </c>
@@ -12754,6 +13685,9 @@
       <c r="A77" s="91" t="s">
         <v>105</v>
       </c>
+      <c r="C77" s="512">
+        <v>23</v>
+      </c>
       <c r="D77" s="459">
         <v>0</v>
       </c>
@@ -12787,6 +13721,9 @@
       <c r="A78" s="91" t="s">
         <v>107</v>
       </c>
+      <c r="C78" s="512">
+        <v>24</v>
+      </c>
       <c r="D78" s="459">
         <v>0</v>
       </c>
@@ -12811,6 +13748,9 @@
       <c r="A79" s="91" t="s">
         <v>109</v>
       </c>
+      <c r="C79" s="512">
+        <v>31</v>
+      </c>
       <c r="D79" s="459">
         <v>0</v>
       </c>
@@ -12845,6 +13785,9 @@
       <c r="A80" s="91" t="s">
         <v>111</v>
       </c>
+      <c r="C80" s="512">
+        <v>41</v>
+      </c>
       <c r="D80" s="459">
         <v>0</v>
       </c>
@@ -12879,6 +13822,9 @@
       <c r="A81" s="91" t="s">
         <v>113</v>
       </c>
+      <c r="C81" s="512">
+        <v>42</v>
+      </c>
       <c r="D81" s="459">
         <v>0</v>
       </c>
@@ -12913,6 +13859,9 @@
       <c r="A82" s="91" t="s">
         <v>115</v>
       </c>
+      <c r="C82" s="512">
+        <v>43</v>
+      </c>
       <c r="D82" s="459">
         <v>0</v>
       </c>
@@ -12937,6 +13886,9 @@
       <c r="A83" s="91" t="s">
         <v>117</v>
       </c>
+      <c r="C83" s="512">
+        <v>52</v>
+      </c>
       <c r="D83" s="459">
         <v>0</v>
       </c>
@@ -12964,6 +13916,9 @@
       <c r="A84" s="91" t="s">
         <v>118</v>
       </c>
+      <c r="C84" s="512">
+        <v>71</v>
+      </c>
       <c r="D84" s="459">
         <v>0</v>
       </c>
@@ -12988,6 +13943,9 @@
       <c r="A85" s="91" t="s">
         <v>120</v>
       </c>
+      <c r="C85" s="512">
+        <v>81</v>
+      </c>
       <c r="D85" s="459">
         <v>0</v>
       </c>
@@ -13012,6 +13970,9 @@
       <c r="A86" s="91" t="s">
         <v>122</v>
       </c>
+      <c r="C86" s="512">
+        <v>82</v>
+      </c>
       <c r="D86" s="459">
         <v>0</v>
       </c>
@@ -13036,6 +13997,9 @@
       <c r="A87" s="91" t="s">
         <v>124</v>
       </c>
+      <c r="C87" s="512">
+        <v>90</v>
+      </c>
       <c r="D87" s="459">
         <v>0</v>
       </c>
@@ -13059,6 +14023,9 @@
     <row r="88" spans="1:15">
       <c r="A88" s="91" t="s">
         <v>125</v>
+      </c>
+      <c r="C88" s="512">
+        <v>95</v>
       </c>
       <c r="D88" s="459">
         <v>0</v>
@@ -13112,6 +14079,9 @@
       <c r="A93" s="91" t="s">
         <v>88</v>
       </c>
+      <c r="C93" s="112" t="s">
+        <v>527</v>
+      </c>
       <c r="D93" s="425" t="s">
         <v>485</v>
       </c>
@@ -13123,6 +14093,9 @@
       <c r="A94" s="91" t="s">
         <v>98</v>
       </c>
+      <c r="C94" s="512">
+        <v>11</v>
+      </c>
       <c r="D94" s="461">
         <v>0</v>
       </c>
@@ -13135,6 +14108,9 @@
       <c r="A95" s="91" t="s">
         <v>100</v>
       </c>
+      <c r="C95" s="512">
+        <v>12</v>
+      </c>
       <c r="D95" s="461">
         <v>0</v>
       </c>
@@ -13147,6 +14123,9 @@
       <c r="A96" s="91" t="s">
         <v>101</v>
       </c>
+      <c r="C96" s="512">
+        <v>21</v>
+      </c>
       <c r="D96" s="461">
         <v>0</v>
       </c>
@@ -13171,6 +14150,9 @@
       <c r="A97" s="91" t="s">
         <v>103</v>
       </c>
+      <c r="C97" s="512">
+        <v>22</v>
+      </c>
       <c r="D97" s="461">
         <v>0</v>
       </c>
@@ -13195,6 +14177,9 @@
       <c r="A98" s="91" t="s">
         <v>105</v>
       </c>
+      <c r="C98" s="512">
+        <v>23</v>
+      </c>
       <c r="D98" s="461">
         <v>0</v>
       </c>
@@ -13219,6 +14204,9 @@
       <c r="A99" s="91" t="s">
         <v>107</v>
       </c>
+      <c r="C99" s="512">
+        <v>24</v>
+      </c>
       <c r="D99" s="461">
         <v>0</v>
       </c>
@@ -13246,6 +14234,9 @@
       <c r="A100" s="91" t="s">
         <v>109</v>
       </c>
+      <c r="C100" s="512">
+        <v>31</v>
+      </c>
       <c r="D100" s="461">
         <v>0</v>
       </c>
@@ -13273,6 +14264,9 @@
       <c r="A101" s="91" t="s">
         <v>111</v>
       </c>
+      <c r="C101" s="512">
+        <v>41</v>
+      </c>
       <c r="D101" s="461">
         <v>0</v>
       </c>
@@ -13297,6 +14291,9 @@
       <c r="A102" s="91" t="s">
         <v>113</v>
       </c>
+      <c r="C102" s="512">
+        <v>42</v>
+      </c>
       <c r="D102" s="461">
         <v>0</v>
       </c>
@@ -13321,6 +14318,9 @@
       <c r="A103" s="91" t="s">
         <v>115</v>
       </c>
+      <c r="C103" s="512">
+        <v>43</v>
+      </c>
       <c r="D103" s="461">
         <v>0</v>
       </c>
@@ -13345,6 +14345,9 @@
       <c r="A104" s="91" t="s">
         <v>117</v>
       </c>
+      <c r="C104" s="512">
+        <v>52</v>
+      </c>
       <c r="D104" s="461">
         <v>0</v>
       </c>
@@ -13369,6 +14372,9 @@
       <c r="A105" s="91" t="s">
         <v>118</v>
       </c>
+      <c r="C105" s="512">
+        <v>71</v>
+      </c>
       <c r="D105" s="461">
         <v>0</v>
       </c>
@@ -13393,6 +14399,9 @@
       <c r="A106" s="91" t="s">
         <v>120</v>
       </c>
+      <c r="C106" s="512">
+        <v>81</v>
+      </c>
       <c r="D106" s="461">
         <v>0</v>
       </c>
@@ -13417,6 +14426,9 @@
       <c r="A107" s="91" t="s">
         <v>122</v>
       </c>
+      <c r="C107" s="512">
+        <v>82</v>
+      </c>
       <c r="D107" s="461">
         <v>0</v>
       </c>
@@ -13441,6 +14453,9 @@
       <c r="A108" s="91" t="s">
         <v>124</v>
       </c>
+      <c r="C108" s="512">
+        <v>90</v>
+      </c>
       <c r="D108" s="461">
         <v>0</v>
       </c>
@@ -13464,6 +14479,9 @@
     <row r="109" spans="1:13">
       <c r="A109" s="91" t="s">
         <v>125</v>
+      </c>
+      <c r="C109" s="512">
+        <v>95</v>
       </c>
       <c r="D109" s="461">
         <v>0</v>
@@ -13710,36 +14728,36 @@
       <c r="M8" s="16"/>
     </row>
     <row r="9" spans="1:28">
-      <c r="B9" s="519" t="s">
+      <c r="B9" s="529" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="519"/>
-      <c r="D9" s="519"/>
-      <c r="E9" s="519"/>
-      <c r="F9" s="519"/>
-      <c r="G9" s="519"/>
-      <c r="H9" s="519"/>
-      <c r="I9" s="519"/>
-      <c r="J9" s="519"/>
-      <c r="K9" s="519"/>
-      <c r="L9" s="519"/>
-      <c r="M9" s="519"/>
-      <c r="O9" s="520" t="s">
+      <c r="C9" s="529"/>
+      <c r="D9" s="529"/>
+      <c r="E9" s="529"/>
+      <c r="F9" s="529"/>
+      <c r="G9" s="529"/>
+      <c r="H9" s="529"/>
+      <c r="I9" s="529"/>
+      <c r="J9" s="529"/>
+      <c r="K9" s="529"/>
+      <c r="L9" s="529"/>
+      <c r="M9" s="529"/>
+      <c r="O9" s="530" t="s">
         <v>9</v>
       </c>
-      <c r="P9" s="521"/>
-      <c r="Q9" s="521"/>
-      <c r="R9" s="521"/>
-      <c r="S9" s="521"/>
-      <c r="T9" s="521"/>
-      <c r="U9" s="521"/>
-      <c r="V9" s="521"/>
-      <c r="W9" s="521"/>
-      <c r="X9" s="521"/>
-      <c r="Y9" s="521"/>
-      <c r="Z9" s="521"/>
-      <c r="AA9" s="521"/>
-      <c r="AB9" s="521"/>
+      <c r="P9" s="531"/>
+      <c r="Q9" s="531"/>
+      <c r="R9" s="531"/>
+      <c r="S9" s="531"/>
+      <c r="T9" s="531"/>
+      <c r="U9" s="531"/>
+      <c r="V9" s="531"/>
+      <c r="W9" s="531"/>
+      <c r="X9" s="531"/>
+      <c r="Y9" s="531"/>
+      <c r="Z9" s="531"/>
+      <c r="AA9" s="531"/>
+      <c r="AB9" s="531"/>
     </row>
     <row r="11" spans="1:28" ht="17" thickBot="1">
       <c r="B11" s="17"/>
@@ -13754,25 +14772,25 @@
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
       <c r="M11" s="19"/>
-      <c r="O11" s="522" t="s">
+      <c r="O11" s="532" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="523"/>
-      <c r="Q11" s="524"/>
+      <c r="P11" s="533"/>
+      <c r="Q11" s="534"/>
       <c r="R11" s="20"/>
-      <c r="S11" s="522" t="s">
+      <c r="S11" s="532" t="s">
         <v>11</v>
       </c>
-      <c r="T11" s="523"/>
-      <c r="U11" s="523"/>
-      <c r="V11" s="524"/>
+      <c r="T11" s="533"/>
+      <c r="U11" s="533"/>
+      <c r="V11" s="534"/>
       <c r="W11" s="20"/>
-      <c r="X11" s="522" t="s">
+      <c r="X11" s="532" t="s">
         <v>12</v>
       </c>
-      <c r="Y11" s="523"/>
-      <c r="Z11" s="523"/>
-      <c r="AA11" s="524"/>
+      <c r="Y11" s="533"/>
+      <c r="Z11" s="533"/>
+      <c r="AA11" s="534"/>
     </row>
     <row r="12" spans="1:28" ht="43">
       <c r="B12" s="21" t="s">
@@ -13991,7 +15009,7 @@
       <c r="AB14" s="360"/>
     </row>
     <row r="15" spans="1:28">
-      <c r="A15" s="513" t="s">
+      <c r="A15" s="523" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="362" t="s">
@@ -14084,7 +15102,7 @@
       </c>
     </row>
     <row r="16" spans="1:28">
-      <c r="A16" s="514"/>
+      <c r="A16" s="524"/>
       <c r="B16" s="372" t="s">
         <v>36</v>
       </c>
@@ -14175,7 +15193,7 @@
       </c>
     </row>
     <row r="17" spans="1:28">
-      <c r="A17" s="514"/>
+      <c r="A17" s="524"/>
       <c r="B17" s="383" t="s">
         <v>37</v>
       </c>
@@ -14264,7 +15282,7 @@
       </c>
     </row>
     <row r="18" spans="1:28">
-      <c r="A18" s="514"/>
+      <c r="A18" s="524"/>
       <c r="B18" s="372" t="s">
         <v>39</v>
       </c>
@@ -14353,7 +15371,7 @@
       </c>
     </row>
     <row r="19" spans="1:28">
-      <c r="A19" s="514"/>
+      <c r="A19" s="524"/>
       <c r="B19" s="383" t="s">
         <v>40</v>
       </c>
@@ -14442,7 +15460,7 @@
       </c>
     </row>
     <row r="20" spans="1:28">
-      <c r="A20" s="514"/>
+      <c r="A20" s="524"/>
       <c r="B20" s="372" t="s">
         <v>41</v>
       </c>
@@ -14531,7 +15549,7 @@
       </c>
     </row>
     <row r="21" spans="1:28">
-      <c r="A21" s="514"/>
+      <c r="A21" s="524"/>
       <c r="B21" s="383" t="s">
         <v>42</v>
       </c>
@@ -14620,7 +15638,7 @@
       </c>
     </row>
     <row r="22" spans="1:28">
-      <c r="A22" s="514"/>
+      <c r="A22" s="524"/>
       <c r="B22" s="372" t="s">
         <v>43</v>
       </c>
@@ -14709,7 +15727,7 @@
       </c>
     </row>
     <row r="23" spans="1:28">
-      <c r="A23" s="514"/>
+      <c r="A23" s="524"/>
       <c r="B23" s="383" t="s">
         <v>44</v>
       </c>
@@ -14798,7 +15816,7 @@
       </c>
     </row>
     <row r="24" spans="1:28">
-      <c r="A24" s="514"/>
+      <c r="A24" s="524"/>
       <c r="B24" s="372" t="s">
         <v>45</v>
       </c>
@@ -14887,7 +15905,7 @@
       </c>
     </row>
     <row r="25" spans="1:28">
-      <c r="A25" s="514"/>
+      <c r="A25" s="524"/>
       <c r="B25" s="383" t="s">
         <v>46</v>
       </c>
@@ -14976,7 +15994,7 @@
       </c>
     </row>
     <row r="26" spans="1:28">
-      <c r="A26" s="514"/>
+      <c r="A26" s="524"/>
       <c r="B26" s="372" t="s">
         <v>47</v>
       </c>
@@ -15065,7 +16083,7 @@
       </c>
     </row>
     <row r="27" spans="1:28">
-      <c r="A27" s="514"/>
+      <c r="A27" s="524"/>
       <c r="B27" s="383" t="s">
         <v>48</v>
       </c>
@@ -15154,7 +16172,7 @@
       </c>
     </row>
     <row r="28" spans="1:28">
-      <c r="A28" s="514"/>
+      <c r="A28" s="524"/>
       <c r="B28" s="372" t="s">
         <v>49</v>
       </c>
@@ -15231,7 +16249,7 @@
       </c>
     </row>
     <row r="29" spans="1:28">
-      <c r="A29" s="514"/>
+      <c r="A29" s="524"/>
       <c r="B29" s="383" t="s">
         <v>50</v>
       </c>
@@ -15308,7 +16326,7 @@
       </c>
     </row>
     <row r="30" spans="1:28" ht="17" thickBot="1">
-      <c r="A30" s="515"/>
+      <c r="A30" s="525"/>
       <c r="B30" s="357" t="s">
         <v>51</v>
       </c>
@@ -15385,7 +16403,7 @@
       </c>
     </row>
     <row r="32" spans="1:28" ht="29">
-      <c r="A32" s="516" t="s">
+      <c r="A32" s="526" t="s">
         <v>52</v>
       </c>
       <c r="B32" s="44" t="s">
@@ -15438,7 +16456,7 @@
       <c r="AB32" s="9"/>
     </row>
     <row r="33" spans="1:28">
-      <c r="A33" s="517"/>
+      <c r="A33" s="527"/>
       <c r="B33" s="49" t="s">
         <v>25</v>
       </c>
@@ -15471,7 +16489,7 @@
       <c r="AB33" s="9"/>
     </row>
     <row r="34" spans="1:28">
-      <c r="A34" s="517"/>
+      <c r="A34" s="527"/>
       <c r="B34" s="54" t="s">
         <v>53</v>
       </c>
@@ -15516,7 +16534,7 @@
       <c r="AB34" s="9"/>
     </row>
     <row r="35" spans="1:28">
-      <c r="A35" s="517"/>
+      <c r="A35" s="527"/>
       <c r="B35" s="58" t="s">
         <v>54</v>
       </c>
@@ -15558,7 +16576,7 @@
       <c r="P35" s="7"/>
     </row>
     <row r="36" spans="1:28">
-      <c r="A36" s="515"/>
+      <c r="A36" s="525"/>
       <c r="B36" s="62" t="s">
         <v>66</v>
       </c>
@@ -15787,66 +16805,66 @@
     </row>
     <row r="44" spans="1:28" s="342" customFormat="1" ht="33" customHeight="1">
       <c r="A44" s="496"/>
-      <c r="B44" s="518" t="s">
+      <c r="B44" s="528" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="518"/>
-      <c r="D44" s="518"/>
-      <c r="E44" s="518"/>
-      <c r="F44" s="518"/>
-      <c r="G44" s="518"/>
-      <c r="H44" s="518"/>
-      <c r="I44" s="518"/>
-      <c r="J44" s="518"/>
-      <c r="K44" s="518"/>
-      <c r="L44" s="518"/>
-      <c r="M44" s="518"/>
-      <c r="N44" s="518"/>
-      <c r="O44" s="518"/>
-      <c r="P44" s="518"/>
-      <c r="Q44" s="518"/>
-      <c r="R44" s="518"/>
-      <c r="S44" s="518"/>
-      <c r="T44" s="518"/>
-      <c r="U44" s="518"/>
-      <c r="V44" s="518"/>
-      <c r="W44" s="518"/>
-      <c r="X44" s="518"/>
-      <c r="Y44" s="518"/>
-      <c r="Z44" s="518"/>
-      <c r="AA44" s="518"/>
+      <c r="C44" s="528"/>
+      <c r="D44" s="528"/>
+      <c r="E44" s="528"/>
+      <c r="F44" s="528"/>
+      <c r="G44" s="528"/>
+      <c r="H44" s="528"/>
+      <c r="I44" s="528"/>
+      <c r="J44" s="528"/>
+      <c r="K44" s="528"/>
+      <c r="L44" s="528"/>
+      <c r="M44" s="528"/>
+      <c r="N44" s="528"/>
+      <c r="O44" s="528"/>
+      <c r="P44" s="528"/>
+      <c r="Q44" s="528"/>
+      <c r="R44" s="528"/>
+      <c r="S44" s="528"/>
+      <c r="T44" s="528"/>
+      <c r="U44" s="528"/>
+      <c r="V44" s="528"/>
+      <c r="W44" s="528"/>
+      <c r="X44" s="528"/>
+      <c r="Y44" s="528"/>
+      <c r="Z44" s="528"/>
+      <c r="AA44" s="528"/>
       <c r="AB44" s="496"/>
     </row>
     <row r="45" spans="1:28" s="342" customFormat="1" ht="33" customHeight="1">
       <c r="A45" s="496"/>
-      <c r="B45" s="518" t="s">
+      <c r="B45" s="528" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="518"/>
-      <c r="D45" s="518"/>
-      <c r="E45" s="518"/>
-      <c r="F45" s="518"/>
-      <c r="G45" s="518"/>
-      <c r="H45" s="518"/>
-      <c r="I45" s="518"/>
-      <c r="J45" s="518"/>
-      <c r="K45" s="518"/>
-      <c r="L45" s="518"/>
-      <c r="M45" s="518"/>
-      <c r="N45" s="518"/>
-      <c r="O45" s="518"/>
-      <c r="P45" s="518"/>
-      <c r="Q45" s="518"/>
-      <c r="R45" s="518"/>
-      <c r="S45" s="518"/>
-      <c r="T45" s="518"/>
-      <c r="U45" s="518"/>
-      <c r="V45" s="518"/>
-      <c r="W45" s="518"/>
-      <c r="X45" s="518"/>
-      <c r="Y45" s="518"/>
-      <c r="Z45" s="518"/>
-      <c r="AA45" s="518"/>
+      <c r="C45" s="528"/>
+      <c r="D45" s="528"/>
+      <c r="E45" s="528"/>
+      <c r="F45" s="528"/>
+      <c r="G45" s="528"/>
+      <c r="H45" s="528"/>
+      <c r="I45" s="528"/>
+      <c r="J45" s="528"/>
+      <c r="K45" s="528"/>
+      <c r="L45" s="528"/>
+      <c r="M45" s="528"/>
+      <c r="N45" s="528"/>
+      <c r="O45" s="528"/>
+      <c r="P45" s="528"/>
+      <c r="Q45" s="528"/>
+      <c r="R45" s="528"/>
+      <c r="S45" s="528"/>
+      <c r="T45" s="528"/>
+      <c r="U45" s="528"/>
+      <c r="V45" s="528"/>
+      <c r="W45" s="528"/>
+      <c r="X45" s="528"/>
+      <c r="Y45" s="528"/>
+      <c r="Z45" s="528"/>
+      <c r="AA45" s="528"/>
       <c r="AB45" s="496"/>
     </row>
     <row r="46" spans="1:28">
@@ -16060,39 +17078,39 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="16">
-      <c r="A5" s="526" t="s">
+      <c r="A5" s="536" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="526"/>
-      <c r="C5" s="526"/>
-      <c r="D5" s="526"/>
-      <c r="E5" s="526"/>
-      <c r="F5" s="526"/>
+      <c r="B5" s="536"/>
+      <c r="C5" s="536"/>
+      <c r="D5" s="536"/>
+      <c r="E5" s="536"/>
+      <c r="F5" s="536"/>
       <c r="G5" s="123"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="527" t="s">
+      <c r="A6" s="537" t="s">
         <v>129</v>
       </c>
-      <c r="B6" s="527"/>
-      <c r="C6" s="527"/>
-      <c r="D6" s="527"/>
-      <c r="E6" s="527"/>
-      <c r="F6" s="527"/>
-      <c r="G6" s="527"/>
-      <c r="H6" s="527"/>
+      <c r="B6" s="537"/>
+      <c r="C6" s="537"/>
+      <c r="D6" s="537"/>
+      <c r="E6" s="537"/>
+      <c r="F6" s="537"/>
+      <c r="G6" s="537"/>
+      <c r="H6" s="537"/>
     </row>
     <row r="9" spans="1:8" s="497" customFormat="1" ht="28" customHeight="1">
-      <c r="A9" s="525" t="s">
+      <c r="A9" s="535" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="525"/>
-      <c r="C9" s="525"/>
-      <c r="D9" s="525"/>
-      <c r="E9" s="525"/>
-      <c r="F9" s="525"/>
-      <c r="G9" s="525"/>
-      <c r="H9" s="525"/>
+      <c r="B9" s="535"/>
+      <c r="C9" s="535"/>
+      <c r="D9" s="535"/>
+      <c r="E9" s="535"/>
+      <c r="F9" s="535"/>
+      <c r="G9" s="535"/>
+      <c r="H9" s="535"/>
     </row>
     <row r="11" spans="1:8">
       <c r="B11" s="94"/>
@@ -16124,23 +17142,23 @@
       <c r="F13" s="130" t="s">
         <v>133</v>
       </c>
-      <c r="G13" s="528" t="s">
+      <c r="G13" s="538" t="s">
         <v>134</v>
       </c>
-      <c r="H13" s="529"/>
+      <c r="H13" s="539"/>
     </row>
     <row r="14" spans="1:8">
       <c r="F14" s="131"/>
-      <c r="G14" s="530"/>
-      <c r="H14" s="531"/>
+      <c r="G14" s="540"/>
+      <c r="H14" s="541"/>
     </row>
     <row r="15" spans="1:8">
       <c r="B15" s="94" t="s">
         <v>135</v>
       </c>
       <c r="F15" s="131"/>
-      <c r="G15" s="532"/>
-      <c r="H15" s="533"/>
+      <c r="G15" s="542"/>
+      <c r="H15" s="543"/>
     </row>
     <row r="16" spans="1:8" ht="14">
       <c r="C16" s="132" t="s">
@@ -16176,29 +17194,29 @@
       </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="B19" s="534" t="s">
+      <c r="B19" s="544" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="534"/>
-      <c r="D19" s="534"/>
-      <c r="E19" s="534"/>
-      <c r="F19" s="534"/>
-      <c r="G19" s="534"/>
+      <c r="C19" s="544"/>
+      <c r="D19" s="544"/>
+      <c r="E19" s="544"/>
+      <c r="F19" s="544"/>
+      <c r="G19" s="544"/>
     </row>
     <row r="20" spans="1:8">
       <c r="D20" s="139"/>
     </row>
     <row r="22" spans="1:8" ht="28" customHeight="1">
-      <c r="A22" s="535" t="s">
+      <c r="A22" s="545" t="s">
         <v>138</v>
       </c>
-      <c r="B22" s="535"/>
-      <c r="C22" s="535"/>
-      <c r="D22" s="535"/>
-      <c r="E22" s="535"/>
-      <c r="F22" s="535"/>
-      <c r="G22" s="535"/>
-      <c r="H22" s="535"/>
+      <c r="B22" s="545"/>
+      <c r="C22" s="545"/>
+      <c r="D22" s="545"/>
+      <c r="E22" s="545"/>
+      <c r="F22" s="545"/>
+      <c r="G22" s="545"/>
+      <c r="H22" s="545"/>
     </row>
     <row r="23" spans="1:8">
       <c r="C23" s="140"/>
@@ -16232,16 +17250,16 @@
       <c r="E26" s="142"/>
     </row>
     <row r="27" spans="1:8" ht="28" customHeight="1">
-      <c r="A27" s="525" t="s">
+      <c r="A27" s="535" t="s">
         <v>141</v>
       </c>
-      <c r="B27" s="525"/>
-      <c r="C27" s="525"/>
-      <c r="D27" s="525"/>
-      <c r="E27" s="525"/>
-      <c r="F27" s="525"/>
-      <c r="G27" s="525"/>
-      <c r="H27" s="525"/>
+      <c r="B27" s="535"/>
+      <c r="C27" s="535"/>
+      <c r="D27" s="535"/>
+      <c r="E27" s="535"/>
+      <c r="F27" s="535"/>
+      <c r="G27" s="535"/>
+      <c r="H27" s="535"/>
     </row>
     <row r="28" spans="1:8">
       <c r="D28" s="139"/>
@@ -16327,16 +17345,16 @@
       <c r="C35" s="164"/>
     </row>
     <row r="36" spans="1:8" s="497" customFormat="1" ht="42" customHeight="1">
-      <c r="A36" s="525" t="s">
+      <c r="A36" s="535" t="s">
         <v>147</v>
       </c>
-      <c r="B36" s="525"/>
-      <c r="C36" s="525"/>
-      <c r="D36" s="525"/>
-      <c r="E36" s="525"/>
-      <c r="F36" s="525"/>
-      <c r="G36" s="525"/>
-      <c r="H36" s="525"/>
+      <c r="B36" s="535"/>
+      <c r="C36" s="535"/>
+      <c r="D36" s="535"/>
+      <c r="E36" s="535"/>
+      <c r="F36" s="535"/>
+      <c r="G36" s="535"/>
+      <c r="H36" s="535"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -16441,91 +17459,91 @@
       </c>
     </row>
     <row r="5" spans="1:25" ht="16">
-      <c r="A5" s="526" t="s">
+      <c r="A5" s="536" t="s">
         <v>519</v>
       </c>
-      <c r="B5" s="526"/>
-      <c r="C5" s="526"/>
-      <c r="D5" s="526"/>
-      <c r="E5" s="526"/>
-      <c r="F5" s="526"/>
-      <c r="I5" s="526" t="s">
+      <c r="B5" s="536"/>
+      <c r="C5" s="536"/>
+      <c r="D5" s="536"/>
+      <c r="E5" s="536"/>
+      <c r="F5" s="536"/>
+      <c r="I5" s="536" t="s">
         <v>520</v>
       </c>
-      <c r="J5" s="526"/>
-      <c r="K5" s="526"/>
-      <c r="L5" s="526"/>
-      <c r="M5" s="526"/>
-      <c r="N5" s="526"/>
-      <c r="R5" s="526" t="s">
+      <c r="J5" s="536"/>
+      <c r="K5" s="536"/>
+      <c r="L5" s="536"/>
+      <c r="M5" s="536"/>
+      <c r="N5" s="536"/>
+      <c r="R5" s="536" t="s">
         <v>521</v>
       </c>
-      <c r="S5" s="526"/>
-      <c r="T5" s="526"/>
-      <c r="U5" s="526"/>
-      <c r="V5" s="526"/>
-      <c r="W5" s="526"/>
+      <c r="S5" s="536"/>
+      <c r="T5" s="536"/>
+      <c r="U5" s="536"/>
+      <c r="V5" s="536"/>
+      <c r="W5" s="536"/>
     </row>
     <row r="6" spans="1:25">
-      <c r="A6" s="527" t="s">
+      <c r="A6" s="537" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="527"/>
-      <c r="C6" s="527"/>
-      <c r="D6" s="527"/>
-      <c r="E6" s="527"/>
-      <c r="F6" s="527"/>
-      <c r="G6" s="527"/>
-      <c r="I6" s="527" t="s">
+      <c r="B6" s="537"/>
+      <c r="C6" s="537"/>
+      <c r="D6" s="537"/>
+      <c r="E6" s="537"/>
+      <c r="F6" s="537"/>
+      <c r="G6" s="537"/>
+      <c r="I6" s="537" t="s">
         <v>216</v>
       </c>
-      <c r="J6" s="527"/>
-      <c r="K6" s="527"/>
-      <c r="L6" s="527"/>
-      <c r="M6" s="527"/>
-      <c r="N6" s="527"/>
-      <c r="O6" s="527"/>
-      <c r="R6" s="527" t="s">
+      <c r="J6" s="537"/>
+      <c r="K6" s="537"/>
+      <c r="L6" s="537"/>
+      <c r="M6" s="537"/>
+      <c r="N6" s="537"/>
+      <c r="O6" s="537"/>
+      <c r="R6" s="537" t="s">
         <v>239</v>
       </c>
-      <c r="S6" s="527"/>
-      <c r="T6" s="527"/>
-      <c r="U6" s="527"/>
-      <c r="V6" s="527"/>
-      <c r="W6" s="527"/>
-      <c r="X6" s="527"/>
+      <c r="S6" s="537"/>
+      <c r="T6" s="537"/>
+      <c r="U6" s="537"/>
+      <c r="V6" s="537"/>
+      <c r="W6" s="537"/>
+      <c r="X6" s="537"/>
     </row>
     <row r="9" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A9" s="535" t="s">
+      <c r="A9" s="545" t="s">
         <v>522</v>
       </c>
-      <c r="B9" s="535"/>
-      <c r="C9" s="535"/>
-      <c r="D9" s="535"/>
-      <c r="E9" s="535"/>
-      <c r="F9" s="535"/>
-      <c r="G9" s="535"/>
+      <c r="B9" s="545"/>
+      <c r="C9" s="545"/>
+      <c r="D9" s="545"/>
+      <c r="E9" s="545"/>
+      <c r="F9" s="545"/>
+      <c r="G9" s="545"/>
       <c r="H9" s="493"/>
-      <c r="I9" s="554" t="s">
+      <c r="I9" s="546" t="s">
         <v>217</v>
       </c>
-      <c r="J9" s="535"/>
-      <c r="K9" s="535"/>
-      <c r="L9" s="535"/>
-      <c r="M9" s="535"/>
-      <c r="N9" s="535"/>
-      <c r="O9" s="535"/>
+      <c r="J9" s="545"/>
+      <c r="K9" s="545"/>
+      <c r="L9" s="545"/>
+      <c r="M9" s="545"/>
+      <c r="N9" s="545"/>
+      <c r="O9" s="545"/>
       <c r="P9" s="493"/>
       <c r="Q9" s="493"/>
-      <c r="R9" s="554" t="s">
+      <c r="R9" s="546" t="s">
         <v>217</v>
       </c>
-      <c r="S9" s="535"/>
-      <c r="T9" s="535"/>
-      <c r="U9" s="535"/>
-      <c r="V9" s="535"/>
-      <c r="W9" s="535"/>
-      <c r="X9" s="535"/>
+      <c r="S9" s="545"/>
+      <c r="T9" s="545"/>
+      <c r="U9" s="545"/>
+      <c r="V9" s="545"/>
+      <c r="W9" s="545"/>
+      <c r="X9" s="545"/>
       <c r="Y9" s="494"/>
     </row>
     <row r="10" spans="1:25">
@@ -16576,11 +17594,11 @@
       <c r="D12" s="167" t="s">
         <v>149</v>
       </c>
-      <c r="E12" s="536" t="s">
+      <c r="E12" s="556" t="s">
         <v>150</v>
       </c>
-      <c r="F12" s="537"/>
-      <c r="G12" s="538"/>
+      <c r="F12" s="557"/>
+      <c r="G12" s="558"/>
       <c r="I12" s="490"/>
       <c r="J12" s="484"/>
       <c r="K12" s="484"/>
@@ -16597,9 +17615,9 @@
       <c r="X12" s="484"/>
     </row>
     <row r="13" spans="1:25">
-      <c r="E13" s="539"/>
-      <c r="F13" s="540"/>
-      <c r="G13" s="541"/>
+      <c r="E13" s="559"/>
+      <c r="F13" s="560"/>
+      <c r="G13" s="561"/>
     </row>
     <row r="14" spans="1:25" ht="14">
       <c r="B14" s="132" t="s">
@@ -16608,9 +17626,9 @@
       <c r="C14" s="133" t="s">
         <v>136</v>
       </c>
-      <c r="E14" s="542"/>
-      <c r="F14" s="543"/>
-      <c r="G14" s="544"/>
+      <c r="E14" s="562"/>
+      <c r="F14" s="563"/>
+      <c r="G14" s="564"/>
       <c r="J14" s="132" t="s">
         <v>13</v>
       </c>
@@ -16631,7 +17649,7 @@
       <c r="X14" s="243"/>
     </row>
     <row r="15" spans="1:25">
-      <c r="A15" s="545" t="s">
+      <c r="A15" s="565" t="s">
         <v>151</v>
       </c>
       <c r="B15" s="169" t="s">
@@ -16641,7 +17659,7 @@
         <f>+'MMW Output'!C20</f>
         <v>0</v>
       </c>
-      <c r="I15" s="555" t="s">
+      <c r="I15" s="547" t="s">
         <v>151</v>
       </c>
       <c r="J15" s="169" t="s">
@@ -16651,7 +17669,7 @@
         <f>+'MMW Output'!C20</f>
         <v>0</v>
       </c>
-      <c r="R15" s="555" t="s">
+      <c r="R15" s="547" t="s">
         <v>151</v>
       </c>
       <c r="S15" s="169" t="s">
@@ -16663,7 +17681,7 @@
       </c>
     </row>
     <row r="16" spans="1:25">
-      <c r="A16" s="546"/>
+      <c r="A16" s="566"/>
       <c r="B16" s="171" t="s">
         <v>36</v>
       </c>
@@ -16671,7 +17689,7 @@
         <f>+'MMW Output'!C21</f>
         <v>0</v>
       </c>
-      <c r="I16" s="556"/>
+      <c r="I16" s="548"/>
       <c r="J16" s="171" t="s">
         <v>36</v>
       </c>
@@ -16679,7 +17697,7 @@
         <f>+'MMW Output'!C21</f>
         <v>0</v>
       </c>
-      <c r="R16" s="556"/>
+      <c r="R16" s="548"/>
       <c r="S16" s="171" t="s">
         <v>36</v>
       </c>
@@ -16689,7 +17707,7 @@
       </c>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="546"/>
+      <c r="A17" s="566"/>
       <c r="B17" s="173" t="s">
         <v>37</v>
       </c>
@@ -16697,7 +17715,7 @@
         <f>+'MMW Output'!C22</f>
         <v>0</v>
       </c>
-      <c r="I17" s="556"/>
+      <c r="I17" s="548"/>
       <c r="J17" s="173" t="s">
         <v>37</v>
       </c>
@@ -16705,7 +17723,7 @@
         <f>+'MMW Output'!C22</f>
         <v>0</v>
       </c>
-      <c r="R17" s="556"/>
+      <c r="R17" s="548"/>
       <c r="S17" s="173" t="s">
         <v>37</v>
       </c>
@@ -16715,7 +17733,7 @@
       </c>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="546"/>
+      <c r="A18" s="566"/>
       <c r="B18" s="171" t="s">
         <v>39</v>
       </c>
@@ -16723,7 +17741,7 @@
         <f>+'MMW Output'!C23</f>
         <v>0</v>
       </c>
-      <c r="I18" s="556"/>
+      <c r="I18" s="548"/>
       <c r="J18" s="171" t="s">
         <v>39</v>
       </c>
@@ -16731,7 +17749,7 @@
         <f>+'MMW Output'!C23</f>
         <v>0</v>
       </c>
-      <c r="R18" s="556"/>
+      <c r="R18" s="548"/>
       <c r="S18" s="171" t="s">
         <v>39</v>
       </c>
@@ -16741,7 +17759,7 @@
       </c>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="546"/>
+      <c r="A19" s="566"/>
       <c r="B19" s="173" t="s">
         <v>40</v>
       </c>
@@ -16749,7 +17767,7 @@
         <f>+'MMW Output'!C24</f>
         <v>0</v>
       </c>
-      <c r="I19" s="556"/>
+      <c r="I19" s="548"/>
       <c r="J19" s="173" t="s">
         <v>40</v>
       </c>
@@ -16757,7 +17775,7 @@
         <f>+'MMW Output'!C24</f>
         <v>0</v>
       </c>
-      <c r="R19" s="556"/>
+      <c r="R19" s="548"/>
       <c r="S19" s="173" t="s">
         <v>40</v>
       </c>
@@ -16767,7 +17785,7 @@
       </c>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="546"/>
+      <c r="A20" s="566"/>
       <c r="B20" s="171" t="s">
         <v>41</v>
       </c>
@@ -16775,7 +17793,7 @@
         <f>+'MMW Output'!C25</f>
         <v>0</v>
       </c>
-      <c r="I20" s="556"/>
+      <c r="I20" s="548"/>
       <c r="J20" s="171" t="s">
         <v>41</v>
       </c>
@@ -16783,7 +17801,7 @@
         <f>+'MMW Output'!C25</f>
         <v>0</v>
       </c>
-      <c r="R20" s="556"/>
+      <c r="R20" s="548"/>
       <c r="S20" s="171" t="s">
         <v>41</v>
       </c>
@@ -16793,7 +17811,7 @@
       </c>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="546"/>
+      <c r="A21" s="566"/>
       <c r="B21" s="173" t="s">
         <v>42</v>
       </c>
@@ -16801,7 +17819,7 @@
         <f>+'MMW Output'!C26</f>
         <v>0</v>
       </c>
-      <c r="I21" s="556"/>
+      <c r="I21" s="548"/>
       <c r="J21" s="173" t="s">
         <v>42</v>
       </c>
@@ -16809,7 +17827,7 @@
         <f>+'MMW Output'!C26</f>
         <v>0</v>
       </c>
-      <c r="R21" s="556"/>
+      <c r="R21" s="548"/>
       <c r="S21" s="173" t="s">
         <v>42</v>
       </c>
@@ -16819,7 +17837,7 @@
       </c>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="546"/>
+      <c r="A22" s="566"/>
       <c r="B22" s="171" t="s">
         <v>43</v>
       </c>
@@ -16827,7 +17845,7 @@
         <f>+'MMW Output'!C27</f>
         <v>0</v>
       </c>
-      <c r="I22" s="556"/>
+      <c r="I22" s="548"/>
       <c r="J22" s="171" t="s">
         <v>43</v>
       </c>
@@ -16835,7 +17853,7 @@
         <f>+'MMW Output'!C27</f>
         <v>0</v>
       </c>
-      <c r="R22" s="556"/>
+      <c r="R22" s="548"/>
       <c r="S22" s="171" t="s">
         <v>43</v>
       </c>
@@ -16845,7 +17863,7 @@
       </c>
     </row>
     <row r="23" spans="1:20">
-      <c r="A23" s="546"/>
+      <c r="A23" s="566"/>
       <c r="B23" s="173" t="s">
         <v>44</v>
       </c>
@@ -16853,7 +17871,7 @@
         <f>+'MMW Output'!C28</f>
         <v>0</v>
       </c>
-      <c r="I23" s="556"/>
+      <c r="I23" s="548"/>
       <c r="J23" s="173" t="s">
         <v>44</v>
       </c>
@@ -16861,7 +17879,7 @@
         <f>+'MMW Output'!C28</f>
         <v>0</v>
       </c>
-      <c r="R23" s="556"/>
+      <c r="R23" s="548"/>
       <c r="S23" s="173" t="s">
         <v>44</v>
       </c>
@@ -16871,7 +17889,7 @@
       </c>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="546"/>
+      <c r="A24" s="566"/>
       <c r="B24" s="171" t="s">
         <v>45</v>
       </c>
@@ -16879,7 +17897,7 @@
         <f>+'MMW Output'!C29</f>
         <v>0</v>
       </c>
-      <c r="I24" s="556"/>
+      <c r="I24" s="548"/>
       <c r="J24" s="171" t="s">
         <v>45</v>
       </c>
@@ -16887,7 +17905,7 @@
         <f>+'MMW Output'!C29</f>
         <v>0</v>
       </c>
-      <c r="R24" s="556"/>
+      <c r="R24" s="548"/>
       <c r="S24" s="171" t="s">
         <v>45</v>
       </c>
@@ -16897,7 +17915,7 @@
       </c>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="546"/>
+      <c r="A25" s="566"/>
       <c r="B25" s="173" t="s">
         <v>46</v>
       </c>
@@ -16905,7 +17923,7 @@
         <f>+'MMW Output'!C30</f>
         <v>0</v>
       </c>
-      <c r="I25" s="556"/>
+      <c r="I25" s="548"/>
       <c r="J25" s="173" t="s">
         <v>46</v>
       </c>
@@ -16913,7 +17931,7 @@
         <f>+'MMW Output'!C30</f>
         <v>0</v>
       </c>
-      <c r="R25" s="556"/>
+      <c r="R25" s="548"/>
       <c r="S25" s="173" t="s">
         <v>46</v>
       </c>
@@ -16923,7 +17941,7 @@
       </c>
     </row>
     <row r="26" spans="1:20">
-      <c r="A26" s="546"/>
+      <c r="A26" s="566"/>
       <c r="B26" s="171" t="s">
         <v>47</v>
       </c>
@@ -16931,7 +17949,7 @@
         <f>+'MMW Output'!C31</f>
         <v>0</v>
       </c>
-      <c r="I26" s="556"/>
+      <c r="I26" s="548"/>
       <c r="J26" s="171" t="s">
         <v>47</v>
       </c>
@@ -16939,7 +17957,7 @@
         <f>+'MMW Output'!C31</f>
         <v>0</v>
       </c>
-      <c r="R26" s="556"/>
+      <c r="R26" s="548"/>
       <c r="S26" s="171" t="s">
         <v>47</v>
       </c>
@@ -16949,7 +17967,7 @@
       </c>
     </row>
     <row r="27" spans="1:20">
-      <c r="A27" s="546"/>
+      <c r="A27" s="566"/>
       <c r="B27" s="173" t="s">
         <v>48</v>
       </c>
@@ -16957,7 +17975,7 @@
         <f>+'MMW Output'!C32</f>
         <v>0</v>
       </c>
-      <c r="I27" s="556"/>
+      <c r="I27" s="548"/>
       <c r="J27" s="173" t="s">
         <v>48</v>
       </c>
@@ -16965,7 +17983,7 @@
         <f>+'MMW Output'!C32</f>
         <v>0</v>
       </c>
-      <c r="R27" s="556"/>
+      <c r="R27" s="548"/>
       <c r="S27" s="173" t="s">
         <v>48</v>
       </c>
@@ -16975,7 +17993,7 @@
       </c>
     </row>
     <row r="28" spans="1:20">
-      <c r="A28" s="546"/>
+      <c r="A28" s="566"/>
       <c r="B28" s="171" t="s">
         <v>49</v>
       </c>
@@ -16983,7 +18001,7 @@
         <f>+'MMW Output'!C33</f>
         <v>0</v>
       </c>
-      <c r="I28" s="556"/>
+      <c r="I28" s="548"/>
       <c r="J28" s="171" t="s">
         <v>49</v>
       </c>
@@ -16991,7 +18009,7 @@
         <f>+'MMW Output'!C33</f>
         <v>0</v>
       </c>
-      <c r="R28" s="556"/>
+      <c r="R28" s="548"/>
       <c r="S28" s="171" t="s">
         <v>49</v>
       </c>
@@ -17001,7 +18019,7 @@
       </c>
     </row>
     <row r="29" spans="1:20">
-      <c r="A29" s="546"/>
+      <c r="A29" s="566"/>
       <c r="B29" s="173" t="s">
         <v>50</v>
       </c>
@@ -17009,7 +18027,7 @@
         <f>+'MMW Output'!C34</f>
         <v>0</v>
       </c>
-      <c r="I29" s="556"/>
+      <c r="I29" s="548"/>
       <c r="J29" s="173" t="s">
         <v>50</v>
       </c>
@@ -17017,7 +18035,7 @@
         <f>+'MMW Output'!C34</f>
         <v>0</v>
       </c>
-      <c r="R29" s="556"/>
+      <c r="R29" s="548"/>
       <c r="S29" s="173" t="s">
         <v>50</v>
       </c>
@@ -17027,7 +18045,7 @@
       </c>
     </row>
     <row r="30" spans="1:20">
-      <c r="A30" s="547"/>
+      <c r="A30" s="567"/>
       <c r="B30" s="175" t="s">
         <v>51</v>
       </c>
@@ -17035,7 +18053,7 @@
         <f>+'MMW Output'!C35</f>
         <v>0</v>
       </c>
-      <c r="I30" s="557"/>
+      <c r="I30" s="549"/>
       <c r="J30" s="175" t="s">
         <v>51</v>
       </c>
@@ -17043,7 +18061,7 @@
         <f>+'MMW Output'!C35</f>
         <v>0</v>
       </c>
-      <c r="R30" s="557"/>
+      <c r="R30" s="549"/>
       <c r="S30" s="175" t="s">
         <v>51</v>
       </c>
@@ -17081,36 +18099,36 @@
       </c>
     </row>
     <row r="34" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A34" s="535" t="s">
+      <c r="A34" s="545" t="s">
         <v>153</v>
       </c>
-      <c r="B34" s="535"/>
-      <c r="C34" s="535"/>
-      <c r="D34" s="535"/>
-      <c r="E34" s="535"/>
-      <c r="F34" s="535"/>
-      <c r="G34" s="535"/>
+      <c r="B34" s="545"/>
+      <c r="C34" s="545"/>
+      <c r="D34" s="545"/>
+      <c r="E34" s="545"/>
+      <c r="F34" s="545"/>
+      <c r="G34" s="545"/>
       <c r="H34" s="493"/>
-      <c r="I34" s="554" t="s">
+      <c r="I34" s="546" t="s">
         <v>218</v>
       </c>
-      <c r="J34" s="535"/>
-      <c r="K34" s="535"/>
-      <c r="L34" s="535"/>
-      <c r="M34" s="535"/>
-      <c r="N34" s="535"/>
-      <c r="O34" s="535"/>
+      <c r="J34" s="545"/>
+      <c r="K34" s="545"/>
+      <c r="L34" s="545"/>
+      <c r="M34" s="545"/>
+      <c r="N34" s="545"/>
+      <c r="O34" s="545"/>
       <c r="P34" s="493"/>
       <c r="Q34" s="493"/>
-      <c r="R34" s="554" t="s">
+      <c r="R34" s="546" t="s">
         <v>240</v>
       </c>
-      <c r="S34" s="535"/>
-      <c r="T34" s="535"/>
-      <c r="U34" s="535"/>
-      <c r="V34" s="535"/>
-      <c r="W34" s="535"/>
-      <c r="X34" s="535"/>
+      <c r="S34" s="545"/>
+      <c r="T34" s="545"/>
+      <c r="U34" s="545"/>
+      <c r="V34" s="545"/>
+      <c r="W34" s="545"/>
+      <c r="X34" s="545"/>
       <c r="Y34" s="494"/>
     </row>
     <row r="35" spans="1:25">
@@ -17197,39 +18215,39 @@
       <c r="U39" s="142"/>
     </row>
     <row r="40" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A40" s="535" t="str">
+      <c r="A40" s="545" t="str">
         <f>CONCATENATE("Step 3. Sum the total acres in the ", 'MMW Output'!C13," watershed.")</f>
         <v>Step 3. Sum the total acres in the Skippack watershed.</v>
       </c>
-      <c r="B40" s="535"/>
-      <c r="C40" s="535"/>
-      <c r="D40" s="535"/>
-      <c r="E40" s="535"/>
-      <c r="F40" s="535"/>
-      <c r="G40" s="535"/>
+      <c r="B40" s="545"/>
+      <c r="C40" s="545"/>
+      <c r="D40" s="545"/>
+      <c r="E40" s="545"/>
+      <c r="F40" s="545"/>
+      <c r="G40" s="545"/>
       <c r="H40" s="493"/>
-      <c r="I40" s="554" t="str">
+      <c r="I40" s="546" t="str">
         <f>CONCATENATE("Step 3. Sum the total acres in the ", 'MMW Output'!C13," watershed.")</f>
         <v>Step 3. Sum the total acres in the Skippack watershed.</v>
       </c>
-      <c r="J40" s="535"/>
-      <c r="K40" s="535"/>
-      <c r="L40" s="535"/>
-      <c r="M40" s="535"/>
-      <c r="N40" s="535"/>
-      <c r="O40" s="535"/>
+      <c r="J40" s="545"/>
+      <c r="K40" s="545"/>
+      <c r="L40" s="545"/>
+      <c r="M40" s="545"/>
+      <c r="N40" s="545"/>
+      <c r="O40" s="545"/>
       <c r="P40" s="493"/>
       <c r="Q40" s="493"/>
-      <c r="R40" s="554" t="str">
+      <c r="R40" s="546" t="str">
         <f>CONCATENATE("Step 3. Sum the total acres in the ", 'MMW Output'!C13," watershed.")</f>
         <v>Step 3. Sum the total acres in the Skippack watershed.</v>
       </c>
-      <c r="S40" s="535"/>
-      <c r="T40" s="535"/>
-      <c r="U40" s="535"/>
-      <c r="V40" s="535"/>
-      <c r="W40" s="535"/>
-      <c r="X40" s="535"/>
+      <c r="S40" s="545"/>
+      <c r="T40" s="545"/>
+      <c r="U40" s="545"/>
+      <c r="V40" s="545"/>
+      <c r="W40" s="545"/>
+      <c r="X40" s="545"/>
       <c r="Y40" s="494"/>
     </row>
     <row r="41" spans="1:25">
@@ -17310,36 +18328,36 @@
       <c r="U44" s="142"/>
     </row>
     <row r="45" spans="1:25" s="495" customFormat="1" ht="58" customHeight="1">
-      <c r="A45" s="535" t="s">
+      <c r="A45" s="545" t="s">
         <v>156</v>
       </c>
-      <c r="B45" s="535"/>
-      <c r="C45" s="535"/>
-      <c r="D45" s="535"/>
-      <c r="E45" s="535"/>
-      <c r="F45" s="535"/>
-      <c r="G45" s="535"/>
+      <c r="B45" s="545"/>
+      <c r="C45" s="545"/>
+      <c r="D45" s="545"/>
+      <c r="E45" s="545"/>
+      <c r="F45" s="545"/>
+      <c r="G45" s="545"/>
       <c r="H45" s="493"/>
-      <c r="I45" s="554" t="s">
+      <c r="I45" s="546" t="s">
         <v>220</v>
       </c>
-      <c r="J45" s="535"/>
-      <c r="K45" s="535"/>
-      <c r="L45" s="535"/>
-      <c r="M45" s="535"/>
-      <c r="N45" s="535"/>
-      <c r="O45" s="535"/>
+      <c r="J45" s="545"/>
+      <c r="K45" s="545"/>
+      <c r="L45" s="545"/>
+      <c r="M45" s="545"/>
+      <c r="N45" s="545"/>
+      <c r="O45" s="545"/>
       <c r="P45" s="493"/>
       <c r="Q45" s="493"/>
-      <c r="R45" s="554" t="s">
+      <c r="R45" s="546" t="s">
         <v>220</v>
       </c>
-      <c r="S45" s="535"/>
-      <c r="T45" s="535"/>
-      <c r="U45" s="535"/>
-      <c r="V45" s="535"/>
-      <c r="W45" s="535"/>
-      <c r="X45" s="535"/>
+      <c r="S45" s="545"/>
+      <c r="T45" s="545"/>
+      <c r="U45" s="545"/>
+      <c r="V45" s="545"/>
+      <c r="W45" s="545"/>
+      <c r="X45" s="545"/>
       <c r="Y45" s="494"/>
     </row>
     <row r="46" spans="1:25">
@@ -17571,36 +18589,36 @@
       </c>
     </row>
     <row r="54" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A54" s="535" t="s">
+      <c r="A54" s="545" t="s">
         <v>167</v>
       </c>
-      <c r="B54" s="535"/>
-      <c r="C54" s="535"/>
-      <c r="D54" s="535"/>
-      <c r="E54" s="535"/>
-      <c r="F54" s="535"/>
-      <c r="G54" s="535"/>
+      <c r="B54" s="545"/>
+      <c r="C54" s="545"/>
+      <c r="D54" s="545"/>
+      <c r="E54" s="545"/>
+      <c r="F54" s="545"/>
+      <c r="G54" s="545"/>
       <c r="H54" s="493"/>
-      <c r="I54" s="554" t="s">
+      <c r="I54" s="546" t="s">
         <v>221</v>
       </c>
-      <c r="J54" s="535"/>
-      <c r="K54" s="535"/>
-      <c r="L54" s="535"/>
-      <c r="M54" s="535"/>
-      <c r="N54" s="535"/>
-      <c r="O54" s="535"/>
+      <c r="J54" s="545"/>
+      <c r="K54" s="545"/>
+      <c r="L54" s="545"/>
+      <c r="M54" s="545"/>
+      <c r="N54" s="545"/>
+      <c r="O54" s="545"/>
       <c r="P54" s="493"/>
       <c r="Q54" s="493"/>
-      <c r="R54" s="554" t="s">
+      <c r="R54" s="546" t="s">
         <v>242</v>
       </c>
-      <c r="S54" s="535"/>
-      <c r="T54" s="535"/>
-      <c r="U54" s="535"/>
-      <c r="V54" s="535"/>
-      <c r="W54" s="535"/>
-      <c r="X54" s="535"/>
+      <c r="S54" s="545"/>
+      <c r="T54" s="545"/>
+      <c r="U54" s="545"/>
+      <c r="V54" s="545"/>
+      <c r="W54" s="545"/>
+      <c r="X54" s="545"/>
       <c r="Y54" s="494"/>
     </row>
     <row r="55" spans="1:25">
@@ -17940,36 +18958,36 @@
       </c>
     </row>
     <row r="68" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A68" s="535" t="s">
+      <c r="A68" s="545" t="s">
         <v>181</v>
       </c>
-      <c r="B68" s="535"/>
-      <c r="C68" s="535"/>
-      <c r="D68" s="535"/>
-      <c r="E68" s="535"/>
-      <c r="F68" s="535"/>
-      <c r="G68" s="535"/>
+      <c r="B68" s="545"/>
+      <c r="C68" s="545"/>
+      <c r="D68" s="545"/>
+      <c r="E68" s="545"/>
+      <c r="F68" s="545"/>
+      <c r="G68" s="545"/>
       <c r="H68" s="493"/>
-      <c r="I68" s="554" t="s">
+      <c r="I68" s="546" t="s">
         <v>227</v>
       </c>
-      <c r="J68" s="535"/>
-      <c r="K68" s="535"/>
-      <c r="L68" s="535"/>
-      <c r="M68" s="535"/>
-      <c r="N68" s="535"/>
-      <c r="O68" s="535"/>
+      <c r="J68" s="545"/>
+      <c r="K68" s="545"/>
+      <c r="L68" s="545"/>
+      <c r="M68" s="545"/>
+      <c r="N68" s="545"/>
+      <c r="O68" s="545"/>
       <c r="P68" s="493"/>
       <c r="Q68" s="493"/>
-      <c r="R68" s="554" t="s">
+      <c r="R68" s="546" t="s">
         <v>248</v>
       </c>
-      <c r="S68" s="535"/>
-      <c r="T68" s="535"/>
-      <c r="U68" s="535"/>
-      <c r="V68" s="535"/>
-      <c r="W68" s="535"/>
-      <c r="X68" s="535"/>
+      <c r="S68" s="545"/>
+      <c r="T68" s="545"/>
+      <c r="U68" s="545"/>
+      <c r="V68" s="545"/>
+      <c r="W68" s="545"/>
+      <c r="X68" s="545"/>
       <c r="Y68" s="494"/>
     </row>
     <row r="70" spans="1:25">
@@ -18044,36 +19062,36 @@
       </c>
     </row>
     <row r="76" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A76" s="535" t="s">
+      <c r="A76" s="545" t="s">
         <v>183</v>
       </c>
-      <c r="B76" s="535"/>
-      <c r="C76" s="535"/>
-      <c r="D76" s="535"/>
-      <c r="E76" s="535"/>
-      <c r="F76" s="535"/>
-      <c r="G76" s="535"/>
+      <c r="B76" s="545"/>
+      <c r="C76" s="545"/>
+      <c r="D76" s="545"/>
+      <c r="E76" s="545"/>
+      <c r="F76" s="545"/>
+      <c r="G76" s="545"/>
       <c r="H76" s="493"/>
-      <c r="I76" s="554" t="s">
+      <c r="I76" s="546" t="s">
         <v>183</v>
       </c>
-      <c r="J76" s="535"/>
-      <c r="K76" s="535"/>
-      <c r="L76" s="535"/>
-      <c r="M76" s="535"/>
-      <c r="N76" s="535"/>
-      <c r="O76" s="535"/>
+      <c r="J76" s="545"/>
+      <c r="K76" s="545"/>
+      <c r="L76" s="545"/>
+      <c r="M76" s="545"/>
+      <c r="N76" s="545"/>
+      <c r="O76" s="545"/>
       <c r="P76" s="493"/>
       <c r="Q76" s="493"/>
-      <c r="R76" s="554" t="s">
+      <c r="R76" s="546" t="s">
         <v>183</v>
       </c>
-      <c r="S76" s="535"/>
-      <c r="T76" s="535"/>
-      <c r="U76" s="535"/>
-      <c r="V76" s="535"/>
-      <c r="W76" s="535"/>
-      <c r="X76" s="535"/>
+      <c r="S76" s="545"/>
+      <c r="T76" s="545"/>
+      <c r="U76" s="545"/>
+      <c r="V76" s="545"/>
+      <c r="W76" s="545"/>
+      <c r="X76" s="545"/>
       <c r="Y76" s="494"/>
     </row>
     <row r="78" spans="1:25">
@@ -18270,36 +19288,36 @@
       </c>
     </row>
     <row r="85" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A85" s="535" t="s">
+      <c r="A85" s="545" t="s">
         <v>187</v>
       </c>
-      <c r="B85" s="535"/>
-      <c r="C85" s="535"/>
-      <c r="D85" s="535"/>
-      <c r="E85" s="535"/>
-      <c r="F85" s="535"/>
-      <c r="G85" s="535"/>
+      <c r="B85" s="545"/>
+      <c r="C85" s="545"/>
+      <c r="D85" s="545"/>
+      <c r="E85" s="545"/>
+      <c r="F85" s="545"/>
+      <c r="G85" s="545"/>
       <c r="H85" s="493"/>
-      <c r="I85" s="554" t="s">
+      <c r="I85" s="546" t="s">
         <v>187</v>
       </c>
-      <c r="J85" s="535"/>
-      <c r="K85" s="535"/>
-      <c r="L85" s="535"/>
-      <c r="M85" s="535"/>
-      <c r="N85" s="535"/>
-      <c r="O85" s="535"/>
+      <c r="J85" s="545"/>
+      <c r="K85" s="545"/>
+      <c r="L85" s="545"/>
+      <c r="M85" s="545"/>
+      <c r="N85" s="545"/>
+      <c r="O85" s="545"/>
       <c r="P85" s="493"/>
       <c r="Q85" s="493"/>
-      <c r="R85" s="554" t="s">
+      <c r="R85" s="546" t="s">
         <v>187</v>
       </c>
-      <c r="S85" s="535"/>
-      <c r="T85" s="535"/>
-      <c r="U85" s="535"/>
-      <c r="V85" s="535"/>
-      <c r="W85" s="535"/>
-      <c r="X85" s="535"/>
+      <c r="S85" s="545"/>
+      <c r="T85" s="545"/>
+      <c r="U85" s="545"/>
+      <c r="V85" s="545"/>
+      <c r="W85" s="545"/>
+      <c r="X85" s="545"/>
       <c r="Y85" s="494"/>
     </row>
     <row r="87" spans="1:25">
@@ -18487,36 +19505,36 @@
       </c>
     </row>
     <row r="94" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A94" s="535" t="s">
+      <c r="A94" s="545" t="s">
         <v>190</v>
       </c>
-      <c r="B94" s="535"/>
-      <c r="C94" s="535"/>
-      <c r="D94" s="535"/>
-      <c r="E94" s="535"/>
-      <c r="F94" s="535"/>
-      <c r="G94" s="535"/>
+      <c r="B94" s="545"/>
+      <c r="C94" s="545"/>
+      <c r="D94" s="545"/>
+      <c r="E94" s="545"/>
+      <c r="F94" s="545"/>
+      <c r="G94" s="545"/>
       <c r="H94" s="493"/>
-      <c r="I94" s="554" t="s">
+      <c r="I94" s="546" t="s">
         <v>228</v>
       </c>
-      <c r="J94" s="535"/>
-      <c r="K94" s="535"/>
-      <c r="L94" s="535"/>
-      <c r="M94" s="535"/>
-      <c r="N94" s="535"/>
-      <c r="O94" s="535"/>
+      <c r="J94" s="545"/>
+      <c r="K94" s="545"/>
+      <c r="L94" s="545"/>
+      <c r="M94" s="545"/>
+      <c r="N94" s="545"/>
+      <c r="O94" s="545"/>
       <c r="P94" s="493"/>
       <c r="Q94" s="493"/>
-      <c r="R94" s="554" t="s">
+      <c r="R94" s="546" t="s">
         <v>249</v>
       </c>
-      <c r="S94" s="535"/>
-      <c r="T94" s="535"/>
-      <c r="U94" s="535"/>
-      <c r="V94" s="535"/>
-      <c r="W94" s="535"/>
-      <c r="X94" s="535"/>
+      <c r="S94" s="545"/>
+      <c r="T94" s="545"/>
+      <c r="U94" s="545"/>
+      <c r="V94" s="545"/>
+      <c r="W94" s="545"/>
+      <c r="X94" s="545"/>
       <c r="Y94" s="494"/>
     </row>
     <row r="96" spans="1:25" ht="28">
@@ -18643,69 +19661,69 @@
       </c>
     </row>
     <row r="101" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A101" s="535" t="s">
+      <c r="A101" s="545" t="s">
         <v>195</v>
       </c>
-      <c r="B101" s="535"/>
-      <c r="C101" s="535"/>
-      <c r="D101" s="535"/>
-      <c r="E101" s="535"/>
-      <c r="F101" s="535"/>
-      <c r="G101" s="535"/>
+      <c r="B101" s="545"/>
+      <c r="C101" s="545"/>
+      <c r="D101" s="545"/>
+      <c r="E101" s="545"/>
+      <c r="F101" s="545"/>
+      <c r="G101" s="545"/>
       <c r="H101" s="493"/>
-      <c r="I101" s="554" t="s">
+      <c r="I101" s="546" t="s">
         <v>195</v>
       </c>
-      <c r="J101" s="535"/>
-      <c r="K101" s="535"/>
-      <c r="L101" s="535"/>
-      <c r="M101" s="535"/>
-      <c r="N101" s="535"/>
-      <c r="O101" s="535"/>
+      <c r="J101" s="545"/>
+      <c r="K101" s="545"/>
+      <c r="L101" s="545"/>
+      <c r="M101" s="545"/>
+      <c r="N101" s="545"/>
+      <c r="O101" s="545"/>
       <c r="P101" s="493"/>
       <c r="Q101" s="493"/>
-      <c r="R101" s="554" t="s">
+      <c r="R101" s="546" t="s">
         <v>195</v>
       </c>
-      <c r="S101" s="535"/>
-      <c r="T101" s="535"/>
-      <c r="U101" s="535"/>
-      <c r="V101" s="535"/>
-      <c r="W101" s="535"/>
-      <c r="X101" s="535"/>
+      <c r="S101" s="545"/>
+      <c r="T101" s="545"/>
+      <c r="U101" s="545"/>
+      <c r="V101" s="545"/>
+      <c r="W101" s="545"/>
+      <c r="X101" s="545"/>
       <c r="Y101" s="494"/>
     </row>
     <row r="102" spans="1:25">
-      <c r="A102" s="527" t="str">
+      <c r="A102" s="537" t="str">
         <f>CONCATENATE("multiplying the 'Percent of Total Impervious Surfaces' (Step 8) by ",ROUND(C98,2)," pounds (calculated in Step 9):")</f>
         <v>multiplying the 'Percent of Total Impervious Surfaces' (Step 8) by 0 pounds (calculated in Step 9):</v>
       </c>
-      <c r="B102" s="527"/>
-      <c r="C102" s="527"/>
-      <c r="D102" s="527"/>
-      <c r="E102" s="527"/>
-      <c r="F102" s="527"/>
-      <c r="G102" s="527"/>
-      <c r="I102" s="527" t="str">
+      <c r="B102" s="537"/>
+      <c r="C102" s="537"/>
+      <c r="D102" s="537"/>
+      <c r="E102" s="537"/>
+      <c r="F102" s="537"/>
+      <c r="G102" s="537"/>
+      <c r="I102" s="537" t="str">
         <f>CONCATENATE("multiplying the 'Percent of Total Impervious Surfaces' (Step 8) by ",ROUND(K98,2)," pounds (calculated in Step 9):")</f>
         <v>multiplying the 'Percent of Total Impervious Surfaces' (Step 8) by 0 pounds (calculated in Step 9):</v>
       </c>
-      <c r="J102" s="527"/>
-      <c r="K102" s="527"/>
-      <c r="L102" s="527"/>
-      <c r="M102" s="527"/>
-      <c r="N102" s="527"/>
-      <c r="O102" s="527"/>
-      <c r="R102" s="527" t="str">
+      <c r="J102" s="537"/>
+      <c r="K102" s="537"/>
+      <c r="L102" s="537"/>
+      <c r="M102" s="537"/>
+      <c r="N102" s="537"/>
+      <c r="O102" s="537"/>
+      <c r="R102" s="537" t="str">
         <f>CONCATENATE("multiplying the 'Percent of Total Impervious Surfaces' (Step 8) by ",ROUND(T98,2)," pounds (calculated in Step 9):")</f>
         <v>multiplying the 'Percent of Total Impervious Surfaces' (Step 8) by 0 pounds (calculated in Step 9):</v>
       </c>
-      <c r="S102" s="527"/>
-      <c r="T102" s="527"/>
-      <c r="U102" s="527"/>
-      <c r="V102" s="527"/>
-      <c r="W102" s="527"/>
-      <c r="X102" s="527"/>
+      <c r="S102" s="537"/>
+      <c r="T102" s="537"/>
+      <c r="U102" s="537"/>
+      <c r="V102" s="537"/>
+      <c r="W102" s="537"/>
+      <c r="X102" s="537"/>
     </row>
     <row r="103" spans="1:25">
       <c r="A103" s="179"/>
@@ -18761,13 +19779,13 @@
         <f>C88*C$98</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D105" s="548" t="e">
+      <c r="D105" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(C88*100,0)," % x ",ROUND(C$98,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E105" s="549"/>
-      <c r="F105" s="549"/>
-      <c r="G105" s="549"/>
+      <c r="E105" s="551"/>
+      <c r="F105" s="551"/>
+      <c r="G105" s="551"/>
       <c r="J105" s="182" t="s">
         <v>159</v>
       </c>
@@ -18775,13 +19793,13 @@
         <f>K88*K$97</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L105" s="548" t="e">
+      <c r="L105" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(K88*100,0)," % x ",ROUND(K$98,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M105" s="549"/>
-      <c r="N105" s="549"/>
-      <c r="O105" s="549"/>
+      <c r="M105" s="551"/>
+      <c r="N105" s="551"/>
+      <c r="O105" s="551"/>
       <c r="S105" s="182" t="s">
         <v>159</v>
       </c>
@@ -18789,13 +19807,13 @@
         <f>T88*T$98</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U105" s="548" t="e">
+      <c r="U105" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(T88*100,0)," % x ",ROUND(T$98,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V105" s="549"/>
-      <c r="W105" s="549"/>
-      <c r="X105" s="549"/>
+      <c r="V105" s="551"/>
+      <c r="W105" s="551"/>
+      <c r="X105" s="551"/>
     </row>
     <row r="106" spans="1:25">
       <c r="B106" s="187" t="s">
@@ -18805,13 +19823,13 @@
         <f>C89*C$98</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D106" s="550" t="e">
+      <c r="D106" s="552" t="e">
         <f>CONCATENATE("=   [ ",ROUND(C89*100,0)," % x ",ROUND(C$98,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E106" s="551"/>
-      <c r="F106" s="551"/>
-      <c r="G106" s="551"/>
+      <c r="E106" s="553"/>
+      <c r="F106" s="553"/>
+      <c r="G106" s="553"/>
       <c r="J106" s="187" t="s">
         <v>161</v>
       </c>
@@ -18819,13 +19837,13 @@
         <f>K89*K$97</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L106" s="550" t="e">
+      <c r="L106" s="552" t="e">
         <f>CONCATENATE("=   [ ",ROUND(K89*100,0)," % x ",ROUND(K$98,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M106" s="551"/>
-      <c r="N106" s="551"/>
-      <c r="O106" s="551"/>
+      <c r="M106" s="553"/>
+      <c r="N106" s="553"/>
+      <c r="O106" s="553"/>
       <c r="S106" s="187" t="s">
         <v>161</v>
       </c>
@@ -18833,13 +19851,13 @@
         <f>T89*T$98</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U106" s="550" t="e">
+      <c r="U106" s="552" t="e">
         <f>CONCATENATE("=   [ ",ROUND(T89*100,0)," % x ",ROUND(T$98,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V106" s="551"/>
-      <c r="W106" s="551"/>
-      <c r="X106" s="551"/>
+      <c r="V106" s="553"/>
+      <c r="W106" s="553"/>
+      <c r="X106" s="553"/>
     </row>
     <row r="107" spans="1:25">
       <c r="B107" s="182" t="s">
@@ -18849,13 +19867,13 @@
         <f>C90*C$98</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D107" s="548" t="e">
+      <c r="D107" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(C90*100,0)," % x ",ROUND(C$98,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E107" s="549"/>
-      <c r="F107" s="549"/>
-      <c r="G107" s="549"/>
+      <c r="E107" s="551"/>
+      <c r="F107" s="551"/>
+      <c r="G107" s="551"/>
       <c r="J107" s="182" t="s">
         <v>163</v>
       </c>
@@ -18863,13 +19881,13 @@
         <f>K90*K$97</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L107" s="548" t="e">
+      <c r="L107" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(K90*100,0)," % x ",ROUND(K$98,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M107" s="549"/>
-      <c r="N107" s="549"/>
-      <c r="O107" s="549"/>
+      <c r="M107" s="551"/>
+      <c r="N107" s="551"/>
+      <c r="O107" s="551"/>
       <c r="S107" s="182" t="s">
         <v>163</v>
       </c>
@@ -18877,13 +19895,13 @@
         <f>T90*T$98</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U107" s="548" t="e">
+      <c r="U107" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(T90*100,0)," % x ",ROUND(T$98,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V107" s="549"/>
-      <c r="W107" s="549"/>
-      <c r="X107" s="549"/>
+      <c r="V107" s="551"/>
+      <c r="W107" s="551"/>
+      <c r="X107" s="551"/>
     </row>
     <row r="108" spans="1:25">
       <c r="C108" s="226"/>
@@ -18891,69 +19909,69 @@
       <c r="T108" s="226"/>
     </row>
     <row r="110" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A110" s="535" t="s">
+      <c r="A110" s="545" t="s">
         <v>197</v>
       </c>
-      <c r="B110" s="535"/>
-      <c r="C110" s="535"/>
-      <c r="D110" s="535"/>
-      <c r="E110" s="535"/>
-      <c r="F110" s="535"/>
-      <c r="G110" s="535"/>
+      <c r="B110" s="545"/>
+      <c r="C110" s="545"/>
+      <c r="D110" s="545"/>
+      <c r="E110" s="545"/>
+      <c r="F110" s="545"/>
+      <c r="G110" s="545"/>
       <c r="H110" s="493"/>
-      <c r="I110" s="554" t="s">
+      <c r="I110" s="546" t="s">
         <v>197</v>
       </c>
-      <c r="J110" s="535"/>
-      <c r="K110" s="535"/>
-      <c r="L110" s="535"/>
-      <c r="M110" s="535"/>
-      <c r="N110" s="535"/>
-      <c r="O110" s="535"/>
+      <c r="J110" s="545"/>
+      <c r="K110" s="545"/>
+      <c r="L110" s="545"/>
+      <c r="M110" s="545"/>
+      <c r="N110" s="545"/>
+      <c r="O110" s="545"/>
       <c r="P110" s="493"/>
       <c r="Q110" s="493"/>
-      <c r="R110" s="554" t="s">
+      <c r="R110" s="546" t="s">
         <v>197</v>
       </c>
-      <c r="S110" s="535"/>
-      <c r="T110" s="535"/>
-      <c r="U110" s="535"/>
-      <c r="V110" s="535"/>
-      <c r="W110" s="535"/>
-      <c r="X110" s="535"/>
+      <c r="S110" s="545"/>
+      <c r="T110" s="545"/>
+      <c r="U110" s="545"/>
+      <c r="V110" s="545"/>
+      <c r="W110" s="545"/>
+      <c r="X110" s="545"/>
       <c r="Y110" s="494"/>
     </row>
     <row r="111" spans="1:25">
-      <c r="A111" s="527" t="e">
+      <c r="A111" s="537" t="e">
         <f>CONCATENATE("the 'Percent of Area of Developed Lands' (from Step 4) by ",ROUND(C97,2)," pounds (calculated in Step 9):")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="B111" s="527"/>
-      <c r="C111" s="527"/>
-      <c r="D111" s="527"/>
-      <c r="E111" s="527"/>
-      <c r="F111" s="527"/>
-      <c r="G111" s="527"/>
-      <c r="I111" s="527" t="e">
+      <c r="B111" s="537"/>
+      <c r="C111" s="537"/>
+      <c r="D111" s="537"/>
+      <c r="E111" s="537"/>
+      <c r="F111" s="537"/>
+      <c r="G111" s="537"/>
+      <c r="I111" s="537" t="e">
         <f>CONCATENATE("the 'Percent of Area of Developed Lands' (from Step 4) by ",ROUND(K97,2)," pounds (calculated in Step 9):")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J111" s="527"/>
-      <c r="K111" s="527"/>
-      <c r="L111" s="527"/>
-      <c r="M111" s="527"/>
-      <c r="N111" s="527"/>
-      <c r="O111" s="527"/>
-      <c r="R111" s="527" t="e">
+      <c r="J111" s="537"/>
+      <c r="K111" s="537"/>
+      <c r="L111" s="537"/>
+      <c r="M111" s="537"/>
+      <c r="N111" s="537"/>
+      <c r="O111" s="537"/>
+      <c r="R111" s="537" t="e">
         <f>CONCATENATE("the 'Percent of Area of Developed Lands' (from Step 4) by ",ROUND(T97,2)," pounds (calculated in Step 9):")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S111" s="527"/>
-      <c r="T111" s="527"/>
-      <c r="U111" s="527"/>
-      <c r="V111" s="527"/>
-      <c r="W111" s="527"/>
-      <c r="X111" s="527"/>
+      <c r="S111" s="537"/>
+      <c r="T111" s="537"/>
+      <c r="U111" s="537"/>
+      <c r="V111" s="537"/>
+      <c r="W111" s="537"/>
+      <c r="X111" s="537"/>
     </row>
     <row r="113" spans="1:25">
       <c r="B113" s="94" t="s">
@@ -18983,13 +20001,13 @@
         <f>(C48/C$51)*C$97</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D114" s="548" t="e">
+      <c r="D114" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(D48*100,0)," % x ",ROUND(C$97,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E114" s="549"/>
-      <c r="F114" s="549"/>
-      <c r="G114" s="549"/>
+      <c r="E114" s="551"/>
+      <c r="F114" s="551"/>
+      <c r="G114" s="551"/>
       <c r="J114" s="182" t="s">
         <v>159</v>
       </c>
@@ -18997,13 +20015,13 @@
         <f>K48/K$51*K$98</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L114" s="548" t="e">
+      <c r="L114" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(L48*100,0)," % x ",ROUND(K$97,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M114" s="549"/>
-      <c r="N114" s="549"/>
-      <c r="O114" s="549"/>
+      <c r="M114" s="551"/>
+      <c r="N114" s="551"/>
+      <c r="O114" s="551"/>
       <c r="S114" s="182" t="s">
         <v>159</v>
       </c>
@@ -19011,13 +20029,13 @@
         <f>T48/T$51*T$97</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U114" s="548" t="e">
+      <c r="U114" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(U48*100,0)," % x ",ROUND(T$97,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V114" s="549"/>
-      <c r="W114" s="549"/>
-      <c r="X114" s="549"/>
+      <c r="V114" s="551"/>
+      <c r="W114" s="551"/>
+      <c r="X114" s="551"/>
     </row>
     <row r="115" spans="1:25">
       <c r="B115" s="187" t="s">
@@ -19027,13 +20045,13 @@
         <f>(C49/C$51)*C$97</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D115" s="550" t="e">
+      <c r="D115" s="552" t="e">
         <f>CONCATENATE("=   [ ",ROUND(D49*100,0)," % x ",ROUND(C$97,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E115" s="551"/>
-      <c r="F115" s="551"/>
-      <c r="G115" s="551"/>
+      <c r="E115" s="553"/>
+      <c r="F115" s="553"/>
+      <c r="G115" s="553"/>
       <c r="J115" s="187" t="s">
         <v>161</v>
       </c>
@@ -19041,13 +20059,13 @@
         <f>K49/K$51*K$98</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L115" s="550" t="e">
+      <c r="L115" s="552" t="e">
         <f>CONCATENATE("=   [ ",ROUND(L49*100,0)," % x ",ROUND(K$97,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M115" s="551"/>
-      <c r="N115" s="551"/>
-      <c r="O115" s="551"/>
+      <c r="M115" s="553"/>
+      <c r="N115" s="553"/>
+      <c r="O115" s="553"/>
       <c r="S115" s="187" t="s">
         <v>161</v>
       </c>
@@ -19055,13 +20073,13 @@
         <f>T49/T$51*T$97</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U115" s="550" t="e">
+      <c r="U115" s="552" t="e">
         <f>CONCATENATE("=   [ ",ROUND(U49*100,0)," % x ",ROUND(T$97,2)," pounds ]")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V115" s="551"/>
-      <c r="W115" s="551"/>
-      <c r="X115" s="551"/>
+      <c r="V115" s="553"/>
+      <c r="W115" s="553"/>
+      <c r="X115" s="553"/>
     </row>
     <row r="116" spans="1:25">
       <c r="B116" s="182" t="s">
@@ -19071,13 +20089,13 @@
         <f>(C50/C$51)*C$97</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D116" s="548" t="e">
+      <c r="D116" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(D50*100,0)," % x ",ROUND(C$97,2)," pounds ] ")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="E116" s="549"/>
-      <c r="F116" s="549"/>
-      <c r="G116" s="549"/>
+      <c r="E116" s="551"/>
+      <c r="F116" s="551"/>
+      <c r="G116" s="551"/>
       <c r="J116" s="182" t="s">
         <v>163</v>
       </c>
@@ -19085,13 +20103,13 @@
         <f>K50/K$51*K$98</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L116" s="548" t="e">
+      <c r="L116" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(L50*100,0)," % x ",ROUND(K$97,2)," pounds ]  ")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M116" s="549"/>
-      <c r="N116" s="549"/>
-      <c r="O116" s="549"/>
+      <c r="M116" s="551"/>
+      <c r="N116" s="551"/>
+      <c r="O116" s="551"/>
       <c r="S116" s="182" t="s">
         <v>163</v>
       </c>
@@ -19099,45 +20117,45 @@
         <f>T50/T$51*T$97</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="U116" s="548" t="e">
+      <c r="U116" s="550" t="e">
         <f>CONCATENATE("=   [ ",ROUND(U50*100,0)," % x ",ROUND(T$97,2)," pounds ]  ")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="V116" s="549"/>
-      <c r="W116" s="549"/>
-      <c r="X116" s="549"/>
+      <c r="V116" s="551"/>
+      <c r="W116" s="551"/>
+      <c r="X116" s="551"/>
     </row>
     <row r="119" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A119" s="535" t="s">
+      <c r="A119" s="545" t="s">
         <v>199</v>
       </c>
-      <c r="B119" s="535"/>
-      <c r="C119" s="535"/>
-      <c r="D119" s="535"/>
-      <c r="E119" s="535"/>
-      <c r="F119" s="535"/>
-      <c r="G119" s="535"/>
+      <c r="B119" s="545"/>
+      <c r="C119" s="545"/>
+      <c r="D119" s="545"/>
+      <c r="E119" s="545"/>
+      <c r="F119" s="545"/>
+      <c r="G119" s="545"/>
       <c r="H119" s="493"/>
-      <c r="I119" s="554" t="s">
+      <c r="I119" s="546" t="s">
         <v>199</v>
       </c>
-      <c r="J119" s="535"/>
-      <c r="K119" s="535"/>
-      <c r="L119" s="535"/>
-      <c r="M119" s="535"/>
-      <c r="N119" s="535"/>
-      <c r="O119" s="535"/>
+      <c r="J119" s="545"/>
+      <c r="K119" s="545"/>
+      <c r="L119" s="545"/>
+      <c r="M119" s="545"/>
+      <c r="N119" s="545"/>
+      <c r="O119" s="545"/>
       <c r="P119" s="493"/>
       <c r="Q119" s="493"/>
-      <c r="R119" s="554" t="s">
+      <c r="R119" s="546" t="s">
         <v>199</v>
       </c>
-      <c r="S119" s="535"/>
-      <c r="T119" s="535"/>
-      <c r="U119" s="535"/>
-      <c r="V119" s="535"/>
-      <c r="W119" s="535"/>
-      <c r="X119" s="535"/>
+      <c r="S119" s="545"/>
+      <c r="T119" s="545"/>
+      <c r="U119" s="545"/>
+      <c r="V119" s="545"/>
+      <c r="W119" s="545"/>
+      <c r="X119" s="545"/>
       <c r="Y119" s="494"/>
     </row>
     <row r="121" spans="1:25">
@@ -19303,81 +20321,81 @@
       <c r="X124" s="186"/>
     </row>
     <row r="128" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A128" s="535" t="s">
+      <c r="A128" s="545" t="s">
         <v>201</v>
       </c>
-      <c r="B128" s="535"/>
-      <c r="C128" s="535"/>
-      <c r="D128" s="535"/>
-      <c r="E128" s="535"/>
-      <c r="F128" s="535"/>
-      <c r="G128" s="535"/>
+      <c r="B128" s="545"/>
+      <c r="C128" s="545"/>
+      <c r="D128" s="545"/>
+      <c r="E128" s="545"/>
+      <c r="F128" s="545"/>
+      <c r="G128" s="545"/>
       <c r="H128" s="493"/>
-      <c r="I128" s="554" t="s">
+      <c r="I128" s="546" t="s">
         <v>201</v>
       </c>
-      <c r="J128" s="535"/>
-      <c r="K128" s="535"/>
-      <c r="L128" s="535"/>
-      <c r="M128" s="535"/>
-      <c r="N128" s="535"/>
-      <c r="O128" s="535"/>
+      <c r="J128" s="545"/>
+      <c r="K128" s="545"/>
+      <c r="L128" s="545"/>
+      <c r="M128" s="545"/>
+      <c r="N128" s="545"/>
+      <c r="O128" s="545"/>
       <c r="P128" s="493"/>
       <c r="Q128" s="493"/>
-      <c r="R128" s="554" t="s">
+      <c r="R128" s="546" t="s">
         <v>201</v>
       </c>
-      <c r="S128" s="535"/>
-      <c r="T128" s="535"/>
-      <c r="U128" s="535"/>
-      <c r="V128" s="535"/>
-      <c r="W128" s="535"/>
-      <c r="X128" s="535"/>
+      <c r="S128" s="545"/>
+      <c r="T128" s="545"/>
+      <c r="U128" s="545"/>
+      <c r="V128" s="545"/>
+      <c r="W128" s="545"/>
+      <c r="X128" s="545"/>
       <c r="Y128" s="494"/>
     </row>
     <row r="130" spans="1:25" ht="28">
-      <c r="A130" s="552" t="s">
+      <c r="A130" s="554" t="s">
         <v>202</v>
       </c>
-      <c r="B130" s="552"/>
+      <c r="B130" s="554"/>
       <c r="C130" s="229" t="s">
         <v>133</v>
       </c>
       <c r="D130" s="230" t="s">
         <v>203</v>
       </c>
-      <c r="E130" s="553" t="s">
+      <c r="E130" s="555" t="s">
         <v>204</v>
       </c>
-      <c r="F130" s="553"/>
-      <c r="I130" s="552" t="s">
+      <c r="F130" s="555"/>
+      <c r="I130" s="554" t="s">
         <v>234</v>
       </c>
-      <c r="J130" s="552"/>
+      <c r="J130" s="554"/>
       <c r="K130" s="229" t="s">
         <v>133</v>
       </c>
       <c r="L130" s="230" t="s">
         <v>203</v>
       </c>
-      <c r="M130" s="553" t="s">
+      <c r="M130" s="555" t="s">
         <v>235</v>
       </c>
-      <c r="N130" s="553"/>
-      <c r="R130" s="552" t="s">
+      <c r="N130" s="555"/>
+      <c r="R130" s="554" t="s">
         <v>254</v>
       </c>
-      <c r="S130" s="552"/>
+      <c r="S130" s="554"/>
       <c r="T130" s="229" t="s">
         <v>133</v>
       </c>
       <c r="U130" s="230" t="s">
         <v>203</v>
       </c>
-      <c r="V130" s="553" t="s">
+      <c r="V130" s="555" t="s">
         <v>255</v>
       </c>
-      <c r="W130" s="553"/>
+      <c r="W130" s="555"/>
     </row>
     <row r="131" spans="1:25">
       <c r="B131" s="231" t="s">
@@ -19566,36 +20584,36 @@
       <c r="X133" s="186"/>
     </row>
     <row r="137" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A137" s="535" t="s">
+      <c r="A137" s="545" t="s">
         <v>205</v>
       </c>
-      <c r="B137" s="535"/>
-      <c r="C137" s="535"/>
-      <c r="D137" s="535"/>
-      <c r="E137" s="535"/>
-      <c r="F137" s="535"/>
-      <c r="G137" s="535"/>
+      <c r="B137" s="545"/>
+      <c r="C137" s="545"/>
+      <c r="D137" s="545"/>
+      <c r="E137" s="545"/>
+      <c r="F137" s="545"/>
+      <c r="G137" s="545"/>
       <c r="H137" s="493"/>
-      <c r="I137" s="554" t="s">
+      <c r="I137" s="546" t="s">
         <v>205</v>
       </c>
-      <c r="J137" s="535"/>
-      <c r="K137" s="535"/>
-      <c r="L137" s="535"/>
-      <c r="M137" s="535"/>
-      <c r="N137" s="535"/>
-      <c r="O137" s="535"/>
+      <c r="J137" s="545"/>
+      <c r="K137" s="545"/>
+      <c r="L137" s="545"/>
+      <c r="M137" s="545"/>
+      <c r="N137" s="545"/>
+      <c r="O137" s="545"/>
       <c r="P137" s="493"/>
       <c r="Q137" s="493"/>
-      <c r="R137" s="554" t="s">
+      <c r="R137" s="546" t="s">
         <v>205</v>
       </c>
-      <c r="S137" s="535"/>
-      <c r="T137" s="535"/>
-      <c r="U137" s="535"/>
-      <c r="V137" s="535"/>
-      <c r="W137" s="535"/>
-      <c r="X137" s="535"/>
+      <c r="S137" s="545"/>
+      <c r="T137" s="545"/>
+      <c r="U137" s="545"/>
+      <c r="V137" s="545"/>
+      <c r="W137" s="545"/>
+      <c r="X137" s="545"/>
       <c r="Y137" s="494"/>
     </row>
     <row r="139" spans="1:25">
@@ -19810,46 +20828,105 @@
       </c>
     </row>
     <row r="148" spans="1:25" s="495" customFormat="1" ht="28" customHeight="1">
-      <c r="A148" s="535" t="s">
+      <c r="A148" s="545" t="s">
         <v>215</v>
       </c>
-      <c r="B148" s="535"/>
-      <c r="C148" s="535"/>
-      <c r="D148" s="535"/>
-      <c r="E148" s="535"/>
-      <c r="F148" s="535"/>
-      <c r="G148" s="535"/>
+      <c r="B148" s="545"/>
+      <c r="C148" s="545"/>
+      <c r="D148" s="545"/>
+      <c r="E148" s="545"/>
+      <c r="F148" s="545"/>
+      <c r="G148" s="545"/>
       <c r="H148" s="493"/>
-      <c r="I148" s="554" t="s">
+      <c r="I148" s="546" t="s">
         <v>238</v>
       </c>
-      <c r="J148" s="535"/>
-      <c r="K148" s="535"/>
-      <c r="L148" s="535"/>
-      <c r="M148" s="535"/>
-      <c r="N148" s="535"/>
-      <c r="O148" s="535"/>
+      <c r="J148" s="545"/>
+      <c r="K148" s="545"/>
+      <c r="L148" s="545"/>
+      <c r="M148" s="545"/>
+      <c r="N148" s="545"/>
+      <c r="O148" s="545"/>
       <c r="P148" s="493"/>
       <c r="Q148" s="493"/>
-      <c r="R148" s="554" t="s">
+      <c r="R148" s="546" t="s">
         <v>257</v>
       </c>
-      <c r="S148" s="535"/>
-      <c r="T148" s="535"/>
-      <c r="U148" s="535"/>
-      <c r="V148" s="535"/>
-      <c r="W148" s="535"/>
-      <c r="X148" s="535"/>
+      <c r="S148" s="545"/>
+      <c r="T148" s="545"/>
+      <c r="U148" s="545"/>
+      <c r="V148" s="545"/>
+      <c r="W148" s="545"/>
+      <c r="X148" s="545"/>
       <c r="Y148" s="494"/>
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="R40:X40"/>
-    <mergeCell ref="R5:W5"/>
-    <mergeCell ref="R6:X6"/>
-    <mergeCell ref="R9:X9"/>
-    <mergeCell ref="R15:R30"/>
-    <mergeCell ref="R34:X34"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A9:G9"/>
+    <mergeCell ref="E12:G14"/>
+    <mergeCell ref="A15:A30"/>
+    <mergeCell ref="A111:G111"/>
+    <mergeCell ref="A40:G40"/>
+    <mergeCell ref="A45:G45"/>
+    <mergeCell ref="A68:G68"/>
+    <mergeCell ref="A76:G76"/>
+    <mergeCell ref="A94:G94"/>
+    <mergeCell ref="A101:G101"/>
+    <mergeCell ref="A102:G102"/>
+    <mergeCell ref="D105:G105"/>
+    <mergeCell ref="D106:G106"/>
+    <mergeCell ref="D107:G107"/>
+    <mergeCell ref="A110:G110"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A85:G85"/>
+    <mergeCell ref="A148:G148"/>
+    <mergeCell ref="D114:G114"/>
+    <mergeCell ref="D115:G115"/>
+    <mergeCell ref="D116:G116"/>
+    <mergeCell ref="A119:G119"/>
+    <mergeCell ref="A128:G128"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="E130:F130"/>
+    <mergeCell ref="A137:G137"/>
+    <mergeCell ref="I148:O148"/>
+    <mergeCell ref="L115:O115"/>
+    <mergeCell ref="L116:O116"/>
+    <mergeCell ref="I119:O119"/>
+    <mergeCell ref="I128:O128"/>
+    <mergeCell ref="I130:J130"/>
+    <mergeCell ref="M130:N130"/>
+    <mergeCell ref="I137:O137"/>
+    <mergeCell ref="L114:O114"/>
+    <mergeCell ref="I45:O45"/>
+    <mergeCell ref="I68:O68"/>
+    <mergeCell ref="I76:O76"/>
+    <mergeCell ref="I94:O94"/>
+    <mergeCell ref="I101:O101"/>
+    <mergeCell ref="I102:O102"/>
+    <mergeCell ref="L105:O105"/>
+    <mergeCell ref="L106:O106"/>
+    <mergeCell ref="L107:O107"/>
+    <mergeCell ref="I110:O110"/>
+    <mergeCell ref="I111:O111"/>
+    <mergeCell ref="I54:O54"/>
+    <mergeCell ref="I85:O85"/>
+    <mergeCell ref="I40:O40"/>
+    <mergeCell ref="I5:N5"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="I9:O9"/>
+    <mergeCell ref="I15:I30"/>
+    <mergeCell ref="I34:O34"/>
+    <mergeCell ref="R148:X148"/>
+    <mergeCell ref="U115:X115"/>
+    <mergeCell ref="U116:X116"/>
+    <mergeCell ref="R119:X119"/>
+    <mergeCell ref="R128:X128"/>
+    <mergeCell ref="R130:S130"/>
+    <mergeCell ref="V130:W130"/>
+    <mergeCell ref="R137:X137"/>
     <mergeCell ref="U114:X114"/>
     <mergeCell ref="R45:X45"/>
     <mergeCell ref="R68:X68"/>
@@ -19864,71 +20941,12 @@
     <mergeCell ref="R111:X111"/>
     <mergeCell ref="R54:X54"/>
     <mergeCell ref="R85:X85"/>
-    <mergeCell ref="R148:X148"/>
-    <mergeCell ref="U115:X115"/>
-    <mergeCell ref="U116:X116"/>
-    <mergeCell ref="R119:X119"/>
-    <mergeCell ref="R128:X128"/>
-    <mergeCell ref="R130:S130"/>
-    <mergeCell ref="V130:W130"/>
-    <mergeCell ref="R137:X137"/>
-    <mergeCell ref="I40:O40"/>
-    <mergeCell ref="I5:N5"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="I9:O9"/>
-    <mergeCell ref="I15:I30"/>
-    <mergeCell ref="I34:O34"/>
-    <mergeCell ref="L114:O114"/>
-    <mergeCell ref="I45:O45"/>
-    <mergeCell ref="I68:O68"/>
-    <mergeCell ref="I76:O76"/>
-    <mergeCell ref="I94:O94"/>
-    <mergeCell ref="I101:O101"/>
-    <mergeCell ref="I102:O102"/>
-    <mergeCell ref="L105:O105"/>
-    <mergeCell ref="L106:O106"/>
-    <mergeCell ref="L107:O107"/>
-    <mergeCell ref="I110:O110"/>
-    <mergeCell ref="I111:O111"/>
-    <mergeCell ref="I54:O54"/>
-    <mergeCell ref="I85:O85"/>
-    <mergeCell ref="I148:O148"/>
-    <mergeCell ref="L115:O115"/>
-    <mergeCell ref="L116:O116"/>
-    <mergeCell ref="I119:O119"/>
-    <mergeCell ref="I128:O128"/>
-    <mergeCell ref="I130:J130"/>
-    <mergeCell ref="M130:N130"/>
-    <mergeCell ref="I137:O137"/>
-    <mergeCell ref="A148:G148"/>
-    <mergeCell ref="D114:G114"/>
-    <mergeCell ref="D115:G115"/>
-    <mergeCell ref="D116:G116"/>
-    <mergeCell ref="A119:G119"/>
-    <mergeCell ref="A128:G128"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="E130:F130"/>
-    <mergeCell ref="A137:G137"/>
-    <mergeCell ref="A111:G111"/>
-    <mergeCell ref="A40:G40"/>
-    <mergeCell ref="A45:G45"/>
-    <mergeCell ref="A68:G68"/>
-    <mergeCell ref="A76:G76"/>
-    <mergeCell ref="A94:G94"/>
-    <mergeCell ref="A101:G101"/>
-    <mergeCell ref="A102:G102"/>
-    <mergeCell ref="D105:G105"/>
-    <mergeCell ref="D106:G106"/>
-    <mergeCell ref="D107:G107"/>
-    <mergeCell ref="A110:G110"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A85:G85"/>
-    <mergeCell ref="A34:G34"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A9:G9"/>
-    <mergeCell ref="E12:G14"/>
-    <mergeCell ref="A15:A30"/>
+    <mergeCell ref="R40:X40"/>
+    <mergeCell ref="R5:W5"/>
+    <mergeCell ref="R6:X6"/>
+    <mergeCell ref="R9:X9"/>
+    <mergeCell ref="R15:R30"/>
+    <mergeCell ref="R34:X34"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.59718749999999998" top="0.5" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -21939,13 +22957,13 @@
       </c>
     </row>
     <row r="2" spans="1:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="558" t="s">
+      <c r="A2" s="568" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="559"/>
-      <c r="C2" s="559"/>
-      <c r="D2" s="559"/>
-      <c r="E2" s="560"/>
+      <c r="B2" s="569"/>
+      <c r="C2" s="569"/>
+      <c r="D2" s="569"/>
+      <c r="E2" s="570"/>
       <c r="I2" s="273" t="s">
         <v>332</v>
       </c>
@@ -22920,11 +23938,11 @@
       <c r="S26" s="271"/>
     </row>
     <row r="27" spans="1:19" ht="15" customHeight="1">
-      <c r="A27" s="561" t="s">
+      <c r="A27" s="571" t="s">
         <v>356</v>
       </c>
-      <c r="B27" s="562"/>
-      <c r="C27" s="562"/>
+      <c r="B27" s="572"/>
+      <c r="C27" s="572"/>
       <c r="I27" s="271" t="s">
         <v>355</v>
       </c>
@@ -22945,11 +23963,11 @@
       <c r="R27" s="307"/>
     </row>
     <row r="28" spans="1:19" s="297" customFormat="1" ht="15" customHeight="1">
-      <c r="A28" s="563" t="s">
+      <c r="A28" s="573" t="s">
         <v>358</v>
       </c>
-      <c r="B28" s="564"/>
-      <c r="C28" s="564"/>
+      <c r="B28" s="574"/>
+      <c r="C28" s="574"/>
       <c r="D28" s="308"/>
       <c r="E28" s="308"/>
       <c r="G28" s="308"/>
@@ -25268,7 +26286,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -25285,16 +26303,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="331" customFormat="1" ht="24">
-      <c r="F1" s="565" t="s">
+      <c r="F1" s="575" t="s">
         <v>390</v>
       </c>
-      <c r="G1" s="565"/>
-      <c r="H1" s="565"/>
-      <c r="J1" s="565" t="s">
+      <c r="G1" s="575"/>
+      <c r="H1" s="575"/>
+      <c r="J1" s="575" t="s">
         <v>461</v>
       </c>
-      <c r="K1" s="565"/>
-      <c r="L1" s="565"/>
+      <c r="K1" s="575"/>
+      <c r="L1" s="575"/>
     </row>
     <row r="2" spans="1:14" s="4" customFormat="1">
       <c r="F2" s="332" t="s">

</xml_diff>